<commit_message>
Adding CA files and prelim analysis scripts
</commit_message>
<xml_diff>
--- a/ProcessedData/WOS_SciConf_20180531_YeEdited20181113.xlsx
+++ b/ProcessedData/WOS_SciConf_20180531_YeEdited20181113.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Research\ResearchGateCiting\GitRepo201811\rgciting\ProcessedData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\adit\My Documents\RG Citations\rgciting\ProcessedData\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15E23F07-1DD7-43B3-8E81-21F29F24208F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9600" windowHeight="3312"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9600" windowHeight="3312" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WOS_SciConf_20180531 (R1)" sheetId="1" r:id="rId1"/>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11235" uniqueCount="1732">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11235" uniqueCount="1737">
   <si>
     <t>AID</t>
   </si>
@@ -5226,13 +5227,28 @@
   <si>
     <t>Simulation und Erprobung
 in der Fahrzeugentwicklung</t>
+  </si>
+  <si>
+    <t>Computing Science</t>
+  </si>
+  <si>
+    <t>DOI:10.4172/2254-609X.100013</t>
+  </si>
+  <si>
+    <t>Journal of Biomedical Sciences</t>
+  </si>
+  <si>
+    <t>Zdoc</t>
+  </si>
+  <si>
+    <t>https://zdoc.site/history-and-applications-of-hydrogels-journal-of-biomedical-.html</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="26" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -6151,16 +6167,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL332"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="I127" sqref="I127"/>
+      <selection pane="bottomLeft" activeCell="L61" sqref="L61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="7" max="7" width="21.5546875" customWidth="1"/>
     <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
@@ -6176,7 +6192,7 @@
     <col min="22" max="22" width="31.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:38">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -6289,7 +6305,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:38">
       <c r="A2">
         <v>183</v>
       </c>
@@ -6405,7 +6421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:38">
       <c r="A3">
         <v>184</v>
       </c>
@@ -6521,7 +6537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:38">
       <c r="A4">
         <v>187</v>
       </c>
@@ -6637,7 +6653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:38">
       <c r="A5">
         <v>227</v>
       </c>
@@ -6753,7 +6769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:38">
       <c r="A6">
         <v>250</v>
       </c>
@@ -6869,7 +6885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:38">
       <c r="A7">
         <v>338</v>
       </c>
@@ -6985,7 +7001,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:38">
       <c r="A8">
         <v>1</v>
       </c>
@@ -7101,7 +7117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:38">
       <c r="A9">
         <v>251</v>
       </c>
@@ -7217,7 +7233,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:38">
       <c r="A10">
         <v>2</v>
       </c>
@@ -7333,7 +7349,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:38">
       <c r="A11">
         <v>3</v>
       </c>
@@ -7449,7 +7465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:38">
       <c r="A12">
         <v>4</v>
       </c>
@@ -7565,7 +7581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:38">
       <c r="A13">
         <v>5</v>
       </c>
@@ -7681,7 +7697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:38">
       <c r="A14">
         <v>6</v>
       </c>
@@ -7797,7 +7813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:38">
       <c r="A15">
         <v>7</v>
       </c>
@@ -7913,7 +7929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:38">
       <c r="A16">
         <v>253</v>
       </c>
@@ -8029,7 +8045,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:38">
       <c r="A17">
         <v>9</v>
       </c>
@@ -8145,7 +8161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:38">
       <c r="A18">
         <v>10</v>
       </c>
@@ -8261,7 +8277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:38">
       <c r="A19">
         <v>11</v>
       </c>
@@ -8377,7 +8393,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:38">
       <c r="A20">
         <v>12</v>
       </c>
@@ -8493,7 +8509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:38">
       <c r="A21">
         <v>13</v>
       </c>
@@ -8609,7 +8625,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:38">
       <c r="A22">
         <v>14</v>
       </c>
@@ -8725,7 +8741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:38">
       <c r="A23">
         <v>16</v>
       </c>
@@ -8841,7 +8857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:38">
       <c r="A24">
         <v>17</v>
       </c>
@@ -8957,7 +8973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:38">
       <c r="A25">
         <v>254</v>
       </c>
@@ -9073,7 +9089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:38">
       <c r="A26">
         <v>18</v>
       </c>
@@ -9189,7 +9205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:38">
       <c r="A27">
         <v>19</v>
       </c>
@@ -9305,7 +9321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:38">
       <c r="A28">
         <v>20</v>
       </c>
@@ -9421,7 +9437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:38">
       <c r="A29">
         <v>21</v>
       </c>
@@ -9537,7 +9553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:38">
       <c r="A30">
         <v>255</v>
       </c>
@@ -9653,7 +9669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:38">
       <c r="A31">
         <v>22</v>
       </c>
@@ -9769,7 +9785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:38">
       <c r="A32">
         <v>23</v>
       </c>
@@ -9885,7 +9901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:38">
       <c r="A33">
         <v>24</v>
       </c>
@@ -10001,7 +10017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:38">
       <c r="A34">
         <v>25</v>
       </c>
@@ -10117,7 +10133,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:38">
       <c r="A35">
         <v>26</v>
       </c>
@@ -10233,7 +10249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:38">
       <c r="A36">
         <v>27</v>
       </c>
@@ -10349,7 +10365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:38">
       <c r="A37">
         <v>28</v>
       </c>
@@ -10465,7 +10481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:38">
       <c r="A38">
         <v>29</v>
       </c>
@@ -10581,7 +10597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:38">
       <c r="A39">
         <v>30</v>
       </c>
@@ -10697,7 +10713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:38">
       <c r="A40">
         <v>31</v>
       </c>
@@ -10813,7 +10829,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:38">
       <c r="A41">
         <v>32</v>
       </c>
@@ -10929,7 +10945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:38">
       <c r="A42">
         <v>231</v>
       </c>
@@ -11045,7 +11061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:38">
       <c r="A43">
         <v>33</v>
       </c>
@@ -11161,7 +11177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:38">
       <c r="A44">
         <v>34</v>
       </c>
@@ -11277,7 +11293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:38">
       <c r="A45">
         <v>256</v>
       </c>
@@ -11393,7 +11409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:38">
       <c r="A46">
         <v>257</v>
       </c>
@@ -11509,7 +11525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:38">
       <c r="A47">
         <v>258</v>
       </c>
@@ -11625,7 +11641,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:38">
       <c r="A48">
         <v>259</v>
       </c>
@@ -11741,7 +11757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:38">
       <c r="A49">
         <v>35</v>
       </c>
@@ -11857,7 +11873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:38">
       <c r="A50">
         <v>36</v>
       </c>
@@ -11973,7 +11989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:38">
       <c r="A51">
         <v>37</v>
       </c>
@@ -12089,7 +12105,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:38">
       <c r="A52">
         <v>260</v>
       </c>
@@ -12205,7 +12221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:38">
       <c r="A53">
         <v>38</v>
       </c>
@@ -12321,7 +12337,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:38">
       <c r="A54">
         <v>39</v>
       </c>
@@ -12437,7 +12453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:38">
       <c r="A55">
         <v>40</v>
       </c>
@@ -12553,7 +12569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:38">
       <c r="A56">
         <v>41</v>
       </c>
@@ -12669,7 +12685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:38">
       <c r="A57">
         <v>42</v>
       </c>
@@ -12785,7 +12801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:38">
       <c r="A58">
         <v>261</v>
       </c>
@@ -12901,7 +12917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:38">
       <c r="A59">
         <v>43</v>
       </c>
@@ -13017,7 +13033,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:38">
       <c r="A60">
         <v>44</v>
       </c>
@@ -13133,7 +13149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:38">
       <c r="A61">
         <v>45</v>
       </c>
@@ -13141,43 +13157,43 @@
         <v>364</v>
       </c>
       <c r="C61" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D61" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E61" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="F61" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="G61" t="s">
-        <v>45</v>
+        <v>1734</v>
       </c>
       <c r="H61" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="I61" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="J61" t="s">
-        <v>45</v>
+        <v>1735</v>
       </c>
       <c r="K61" t="s">
-        <v>45</v>
+        <v>1736</v>
       </c>
       <c r="L61" t="s">
-        <v>45</v>
+        <v>1733</v>
       </c>
       <c r="M61" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="N61" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="O61" t="s">
-        <v>45</v>
+        <v>1396</v>
       </c>
       <c r="P61" t="s">
         <v>45</v>
@@ -13249,7 +13265,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:38">
       <c r="A62">
         <v>46</v>
       </c>
@@ -13365,7 +13381,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:38">
       <c r="A63">
         <v>47</v>
       </c>
@@ -13481,7 +13497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:38">
       <c r="A64">
         <v>263</v>
       </c>
@@ -13597,7 +13613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:38">
       <c r="A65">
         <v>48</v>
       </c>
@@ -13713,7 +13729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:38">
       <c r="A66">
         <v>49</v>
       </c>
@@ -13829,7 +13845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:38">
       <c r="A67">
         <v>50</v>
       </c>
@@ -13945,7 +13961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:38">
       <c r="A68">
         <v>264</v>
       </c>
@@ -14061,7 +14077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:38">
       <c r="A69">
         <v>265</v>
       </c>
@@ -14177,7 +14193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:38">
       <c r="A70">
         <v>51</v>
       </c>
@@ -14293,7 +14309,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:38">
       <c r="A71">
         <v>266</v>
       </c>
@@ -14409,7 +14425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:38">
       <c r="A72">
         <v>54</v>
       </c>
@@ -14525,7 +14541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:38">
       <c r="A73">
         <v>52</v>
       </c>
@@ -14641,7 +14657,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:38">
       <c r="A74">
         <v>317</v>
       </c>
@@ -14757,7 +14773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:38">
       <c r="A75">
         <v>53</v>
       </c>
@@ -14873,7 +14889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:38">
       <c r="A76">
         <v>56</v>
       </c>
@@ -14989,7 +15005,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:38">
       <c r="A77">
         <v>57</v>
       </c>
@@ -15105,7 +15121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:38">
       <c r="A78">
         <v>58</v>
       </c>
@@ -15221,7 +15237,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="79" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:38">
       <c r="A79">
         <v>267</v>
       </c>
@@ -15337,7 +15353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:38">
       <c r="A80">
         <v>59</v>
       </c>
@@ -15453,7 +15469,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:38">
       <c r="A81">
         <v>60</v>
       </c>
@@ -15569,7 +15585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:38">
       <c r="A82">
         <v>61</v>
       </c>
@@ -15685,7 +15701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:38">
       <c r="A83">
         <v>55</v>
       </c>
@@ -15801,7 +15817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:38">
       <c r="A84">
         <v>268</v>
       </c>
@@ -15917,7 +15933,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="85" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:38">
       <c r="A85">
         <v>269</v>
       </c>
@@ -16033,7 +16049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:38">
       <c r="A86">
         <v>62</v>
       </c>
@@ -16149,7 +16165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:38">
       <c r="A87">
         <v>270</v>
       </c>
@@ -16265,7 +16281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:38">
       <c r="A88">
         <v>63</v>
       </c>
@@ -16381,7 +16397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:38">
       <c r="A89">
         <v>64</v>
       </c>
@@ -16497,7 +16513,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:38">
       <c r="A90">
         <v>271</v>
       </c>
@@ -16613,7 +16629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:38">
       <c r="A91">
         <v>65</v>
       </c>
@@ -16729,7 +16745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:38">
       <c r="A92">
         <v>66</v>
       </c>
@@ -16845,7 +16861,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:38">
       <c r="A93">
         <v>195</v>
       </c>
@@ -16961,7 +16977,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:38">
       <c r="A94">
         <v>67</v>
       </c>
@@ -17077,7 +17093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:38">
       <c r="A95">
         <v>68</v>
       </c>
@@ -17193,7 +17209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:38">
       <c r="A96">
         <v>69</v>
       </c>
@@ -17309,7 +17325,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:38">
       <c r="A97">
         <v>70</v>
       </c>
@@ -17425,7 +17441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:38">
       <c r="A98">
         <v>71</v>
       </c>
@@ -17541,7 +17557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:38">
       <c r="A99">
         <v>72</v>
       </c>
@@ -17657,7 +17673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:38">
       <c r="A100">
         <v>73</v>
       </c>
@@ -17773,7 +17789,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:38">
       <c r="A101">
         <v>272</v>
       </c>
@@ -17889,7 +17905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:38">
       <c r="A102">
         <v>74</v>
       </c>
@@ -18005,7 +18021,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="103" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:38">
       <c r="A103">
         <v>75</v>
       </c>
@@ -18121,7 +18137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:38" ht="15" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:38" ht="15">
       <c r="A104">
         <v>76</v>
       </c>
@@ -18237,7 +18253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:38">
       <c r="A105">
         <v>77</v>
       </c>
@@ -18353,7 +18369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:38">
       <c r="A106">
         <v>78</v>
       </c>
@@ -18469,7 +18485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:38">
       <c r="A107">
         <v>79</v>
       </c>
@@ -18585,7 +18601,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="108" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:38">
       <c r="A108">
         <v>80</v>
       </c>
@@ -18701,7 +18717,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:38">
       <c r="A109" s="6">
         <v>81</v>
       </c>
@@ -18817,7 +18833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:38">
       <c r="A110">
         <v>82</v>
       </c>
@@ -18933,7 +18949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:38">
       <c r="A111">
         <v>83</v>
       </c>
@@ -19049,7 +19065,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:38">
       <c r="A112">
         <v>273</v>
       </c>
@@ -19165,7 +19181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:38">
       <c r="A113">
         <v>84</v>
       </c>
@@ -19281,7 +19297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:38">
       <c r="A114">
         <v>85</v>
       </c>
@@ -19397,7 +19413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:38">
       <c r="A115">
         <v>86</v>
       </c>
@@ -19513,7 +19529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:38">
       <c r="A116">
         <v>87</v>
       </c>
@@ -19629,7 +19645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:38">
       <c r="A117">
         <v>88</v>
       </c>
@@ -19745,7 +19761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:38">
       <c r="A118">
         <v>89</v>
       </c>
@@ -19861,7 +19877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:38">
       <c r="A119">
         <v>90</v>
       </c>
@@ -19977,7 +19993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:38">
       <c r="A120">
         <v>91</v>
       </c>
@@ -20093,7 +20109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:38">
       <c r="A121">
         <v>92</v>
       </c>
@@ -20209,7 +20225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:38">
       <c r="A122">
         <v>93</v>
       </c>
@@ -20325,7 +20341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:38">
       <c r="A123">
         <v>94</v>
       </c>
@@ -20345,7 +20361,7 @@
         <v>39</v>
       </c>
       <c r="G123" t="s">
-        <v>39</v>
+        <v>1732</v>
       </c>
       <c r="H123" t="s">
         <v>1365</v>
@@ -20438,7 +20454,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="124" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:38">
       <c r="A124">
         <v>95</v>
       </c>
@@ -20554,7 +20570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:38">
       <c r="A125">
         <v>126</v>
       </c>
@@ -20670,7 +20686,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="126" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:38">
       <c r="A126">
         <v>96</v>
       </c>
@@ -20786,7 +20802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:38">
       <c r="A127">
         <v>97</v>
       </c>
@@ -20902,7 +20918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:38">
       <c r="A128">
         <v>98</v>
       </c>
@@ -21018,7 +21034,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:38">
       <c r="A129">
         <v>99</v>
       </c>
@@ -21134,7 +21150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:38">
       <c r="A130">
         <v>100</v>
       </c>
@@ -21250,7 +21266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:38">
       <c r="A131">
         <v>101</v>
       </c>
@@ -21366,7 +21382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:38">
       <c r="A132">
         <v>102</v>
       </c>
@@ -21482,7 +21498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:38">
       <c r="A133">
         <v>103</v>
       </c>
@@ -21598,7 +21614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:38">
       <c r="A134">
         <v>104</v>
       </c>
@@ -21714,7 +21730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:38">
       <c r="A135">
         <v>275</v>
       </c>
@@ -21830,7 +21846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:38">
       <c r="A136">
         <v>105</v>
       </c>
@@ -21946,7 +21962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:38">
       <c r="A137">
         <v>106</v>
       </c>
@@ -22062,7 +22078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:38">
       <c r="A138">
         <v>276</v>
       </c>
@@ -22178,7 +22194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:38">
       <c r="A139">
         <v>107</v>
       </c>
@@ -22294,7 +22310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:38">
       <c r="A140">
         <v>108</v>
       </c>
@@ -22410,7 +22426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:38">
       <c r="A141">
         <v>277</v>
       </c>
@@ -22526,7 +22542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:38">
       <c r="A142">
         <v>109</v>
       </c>
@@ -22642,7 +22658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:38">
       <c r="A143">
         <v>110</v>
       </c>
@@ -22758,7 +22774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:38">
       <c r="A144">
         <v>111</v>
       </c>
@@ -22874,7 +22890,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:38">
       <c r="A145">
         <v>112</v>
       </c>
@@ -22990,7 +23006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:38">
       <c r="A146">
         <v>278</v>
       </c>
@@ -23106,7 +23122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:38">
       <c r="A147">
         <v>113</v>
       </c>
@@ -23222,7 +23238,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:38">
       <c r="A148">
         <v>114</v>
       </c>
@@ -23338,7 +23354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:38">
       <c r="A149">
         <v>115</v>
       </c>
@@ -23454,7 +23470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:38">
       <c r="A150">
         <v>116</v>
       </c>
@@ -23570,7 +23586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:38">
       <c r="A151">
         <v>117</v>
       </c>
@@ -23686,7 +23702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:38">
       <c r="A152">
         <v>118</v>
       </c>
@@ -23802,7 +23818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:38">
       <c r="A153">
         <v>279</v>
       </c>
@@ -23918,7 +23934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:38">
       <c r="A154">
         <v>119</v>
       </c>
@@ -24034,7 +24050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:38">
       <c r="A155">
         <v>120</v>
       </c>
@@ -24150,7 +24166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:38">
       <c r="A156">
         <v>280</v>
       </c>
@@ -24266,7 +24282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:38">
       <c r="A157">
         <v>281</v>
       </c>
@@ -24382,7 +24398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:38">
       <c r="A158">
         <v>121</v>
       </c>
@@ -24498,7 +24514,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:38">
       <c r="A159">
         <v>282</v>
       </c>
@@ -24614,7 +24630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:38">
       <c r="A160">
         <v>122</v>
       </c>
@@ -24730,7 +24746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:38">
       <c r="A161">
         <v>128</v>
       </c>
@@ -24846,7 +24862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:38">
       <c r="A162">
         <v>124</v>
       </c>
@@ -24962,7 +24978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:38">
       <c r="A163">
         <v>125</v>
       </c>
@@ -25078,7 +25094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:38">
       <c r="A164">
         <v>127</v>
       </c>
@@ -25194,7 +25210,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:38">
       <c r="A165">
         <v>283</v>
       </c>
@@ -25310,7 +25326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:38">
       <c r="A166">
         <v>284</v>
       </c>
@@ -25426,7 +25442,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:38">
       <c r="A167">
         <v>129</v>
       </c>
@@ -25542,7 +25558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:38">
       <c r="A168">
         <v>130</v>
       </c>
@@ -25658,7 +25674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:38">
       <c r="A169">
         <v>131</v>
       </c>
@@ -25774,7 +25790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:38">
       <c r="A170">
         <v>132</v>
       </c>
@@ -25890,7 +25906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:38">
       <c r="A171">
         <v>285</v>
       </c>
@@ -26006,7 +26022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:38">
       <c r="A172">
         <v>133</v>
       </c>
@@ -26122,7 +26138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:38">
       <c r="A173">
         <v>134</v>
       </c>
@@ -26238,7 +26254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:38">
       <c r="A174">
         <v>135</v>
       </c>
@@ -26354,7 +26370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:38">
       <c r="A175">
         <v>136</v>
       </c>
@@ -26470,7 +26486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:38">
       <c r="A176">
         <v>286</v>
       </c>
@@ -26586,7 +26602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:38">
       <c r="A177">
         <v>138</v>
       </c>
@@ -26702,7 +26718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:38">
       <c r="A178">
         <v>137</v>
       </c>
@@ -26818,7 +26834,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:38">
       <c r="A179">
         <v>139</v>
       </c>
@@ -26934,7 +26950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:38">
       <c r="A180" s="6">
         <v>218</v>
       </c>
@@ -27050,7 +27066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:38">
       <c r="A181">
         <v>287</v>
       </c>
@@ -27166,7 +27182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:38">
       <c r="A182">
         <v>140</v>
       </c>
@@ -27282,7 +27298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:38">
       <c r="A183">
         <v>141</v>
       </c>
@@ -27398,7 +27414,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="184" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:38">
       <c r="A184">
         <v>142</v>
       </c>
@@ -27514,7 +27530,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:38">
       <c r="A185">
         <v>143</v>
       </c>
@@ -27630,7 +27646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:38">
       <c r="A186">
         <v>288</v>
       </c>
@@ -27746,7 +27762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:38">
       <c r="A187">
         <v>289</v>
       </c>
@@ -27862,7 +27878,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:38">
       <c r="A188">
         <v>144</v>
       </c>
@@ -27978,7 +27994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:38">
       <c r="A189">
         <v>145</v>
       </c>
@@ -28094,7 +28110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:38">
       <c r="A190">
         <v>290</v>
       </c>
@@ -28210,7 +28226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:38">
       <c r="A191">
         <v>146</v>
       </c>
@@ -28326,7 +28342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:38">
       <c r="A192">
         <v>147</v>
       </c>
@@ -28442,7 +28458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:38">
       <c r="A193">
         <v>148</v>
       </c>
@@ -28558,7 +28574,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="194" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:38">
       <c r="A194" s="6">
         <v>149</v>
       </c>
@@ -28674,7 +28690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:38">
       <c r="A195">
         <v>150</v>
       </c>
@@ -28790,7 +28806,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="196" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:38">
       <c r="A196">
         <v>151</v>
       </c>
@@ -28906,7 +28922,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="197" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:38">
       <c r="A197">
         <v>152</v>
       </c>
@@ -29022,7 +29038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:38">
       <c r="A198" s="6">
         <v>153</v>
       </c>
@@ -29138,7 +29154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:38">
       <c r="A199">
         <v>291</v>
       </c>
@@ -29254,7 +29270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:38">
       <c r="A200">
         <v>292</v>
       </c>
@@ -29370,7 +29386,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:38">
       <c r="A201">
         <v>293</v>
       </c>
@@ -29486,7 +29502,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:38">
       <c r="A202">
         <v>154</v>
       </c>
@@ -29602,7 +29618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:38">
       <c r="A203">
         <v>294</v>
       </c>
@@ -29718,7 +29734,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:38">
       <c r="A204">
         <v>155</v>
       </c>
@@ -29834,7 +29850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="205" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:38">
       <c r="A205">
         <v>156</v>
       </c>
@@ -29950,7 +29966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:38">
       <c r="A206">
         <v>295</v>
       </c>
@@ -30066,7 +30082,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="207" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:38">
       <c r="A207">
         <v>296</v>
       </c>
@@ -30182,7 +30198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:38">
       <c r="A208">
         <v>157</v>
       </c>
@@ -30298,7 +30314,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:38">
       <c r="A209">
         <v>158</v>
       </c>
@@ -30414,7 +30430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:38">
       <c r="A210">
         <v>159</v>
       </c>
@@ -30530,7 +30546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:38">
       <c r="A211">
         <v>160</v>
       </c>
@@ -30646,7 +30662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:38">
       <c r="A212">
         <v>161</v>
       </c>
@@ -30762,7 +30778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="213" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:38">
       <c r="A213">
         <v>297</v>
       </c>
@@ -30878,7 +30894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="214" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:38">
       <c r="A214">
         <v>298</v>
       </c>
@@ -30994,7 +31010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="215" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:38">
       <c r="A215">
         <v>162</v>
       </c>
@@ -31110,7 +31126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="216" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:38">
       <c r="A216">
         <v>299</v>
       </c>
@@ -31226,7 +31242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="217" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:38">
       <c r="A217">
         <v>164</v>
       </c>
@@ -31342,7 +31358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="218" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:38">
       <c r="A218">
         <v>163</v>
       </c>
@@ -31458,7 +31474,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="219" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:38">
       <c r="A219">
         <v>165</v>
       </c>
@@ -31574,7 +31590,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="220" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:38">
       <c r="A220">
         <v>168</v>
       </c>
@@ -31690,7 +31706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="221" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:38">
       <c r="A221">
         <v>166</v>
       </c>
@@ -31806,7 +31822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="222" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:38">
       <c r="A222">
         <v>300</v>
       </c>
@@ -31922,7 +31938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="223" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:38">
       <c r="A223">
         <v>301</v>
       </c>
@@ -32038,7 +32054,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="224" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:38">
       <c r="A224">
         <v>167</v>
       </c>
@@ -32154,7 +32170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="225" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:38">
       <c r="A225">
         <v>169</v>
       </c>
@@ -32270,7 +32286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="226" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:38">
       <c r="A226">
         <v>170</v>
       </c>
@@ -32386,7 +32402,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:38">
       <c r="A227">
         <v>171</v>
       </c>
@@ -32502,7 +32518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="228" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:38">
       <c r="A228">
         <v>303</v>
       </c>
@@ -32618,7 +32634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="229" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:38">
       <c r="A229">
         <v>172</v>
       </c>
@@ -32734,7 +32750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="230" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:38">
       <c r="A230">
         <v>304</v>
       </c>
@@ -32850,7 +32866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="231" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:38">
       <c r="A231" s="6">
         <v>173</v>
       </c>
@@ -32966,7 +32982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:38">
       <c r="A232">
         <v>174</v>
       </c>
@@ -33082,7 +33098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="233" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:38">
       <c r="A233">
         <v>305</v>
       </c>
@@ -33198,7 +33214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="234" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:38">
       <c r="A234">
         <v>8</v>
       </c>
@@ -33311,7 +33327,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="235" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:38">
       <c r="A235">
         <v>175</v>
       </c>
@@ -33427,7 +33443,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="236" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:38">
       <c r="A236">
         <v>306</v>
       </c>
@@ -33543,7 +33559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="237" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:38">
       <c r="A237">
         <v>176</v>
       </c>
@@ -33659,7 +33675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="238" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:38">
       <c r="A238">
         <v>177</v>
       </c>
@@ -33775,7 +33791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="239" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:38">
       <c r="A239">
         <v>307</v>
       </c>
@@ -33891,7 +33907,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="240" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:38">
       <c r="A240">
         <v>308</v>
       </c>
@@ -34007,7 +34023,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="241" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:38">
       <c r="A241">
         <v>178</v>
       </c>
@@ -34123,7 +34139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="242" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:38">
       <c r="A242">
         <v>179</v>
       </c>
@@ -34239,7 +34255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="243" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:38">
       <c r="A243">
         <v>180</v>
       </c>
@@ -34355,7 +34371,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="244" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:38">
       <c r="A244">
         <v>181</v>
       </c>
@@ -34471,7 +34487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="245" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:38">
       <c r="A245" s="6">
         <v>309</v>
       </c>
@@ -34587,7 +34603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="246" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:38">
       <c r="A246">
         <v>182</v>
       </c>
@@ -34703,7 +34719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="247" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:38">
       <c r="A247">
         <v>310</v>
       </c>
@@ -34819,7 +34835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="248" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:38">
       <c r="A248">
         <v>188</v>
       </c>
@@ -34935,7 +34951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="249" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:38">
       <c r="A249">
         <v>189</v>
       </c>
@@ -35051,7 +35067,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="250" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:38">
       <c r="A250">
         <v>190</v>
       </c>
@@ -35167,7 +35183,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="251" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:38">
       <c r="A251">
         <v>191</v>
       </c>
@@ -35283,7 +35299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="252" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:38">
       <c r="A252">
         <v>311</v>
       </c>
@@ -35399,7 +35415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="253" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:38">
       <c r="A253">
         <v>192</v>
       </c>
@@ -35512,7 +35528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="254" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:38">
       <c r="A254">
         <v>312</v>
       </c>
@@ -35628,7 +35644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="255" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:38">
       <c r="A255" s="6">
         <v>313</v>
       </c>
@@ -35744,7 +35760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="256" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:38">
       <c r="A256">
         <v>193</v>
       </c>
@@ -35860,7 +35876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="257" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:38">
       <c r="A257">
         <v>314</v>
       </c>
@@ -35976,7 +35992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="258" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:38">
       <c r="A258">
         <v>315</v>
       </c>
@@ -36092,7 +36108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="259" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:38">
       <c r="A259">
         <v>194</v>
       </c>
@@ -36208,7 +36224,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="260" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:38" ht="15.6">
       <c r="A260">
         <v>196</v>
       </c>
@@ -36324,7 +36340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="261" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:38">
       <c r="A261">
         <v>197</v>
       </c>
@@ -36440,7 +36456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="262" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:38">
       <c r="A262">
         <v>198</v>
       </c>
@@ -36556,7 +36572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="263" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:38">
       <c r="A263">
         <v>199</v>
       </c>
@@ -36672,7 +36688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="264" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:38">
       <c r="A264">
         <v>200</v>
       </c>
@@ -36788,7 +36804,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="265" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:38">
       <c r="A265">
         <v>201</v>
       </c>
@@ -36901,7 +36917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="266" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:38">
       <c r="A266">
         <v>316</v>
       </c>
@@ -37017,7 +37033,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="267" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:38">
       <c r="A267">
         <v>202</v>
       </c>
@@ -37133,7 +37149,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="268" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:38">
       <c r="A268">
         <v>203</v>
       </c>
@@ -37249,7 +37265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="269" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:38">
       <c r="A269">
         <v>204</v>
       </c>
@@ -37365,7 +37381,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="270" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:38">
       <c r="A270">
         <v>318</v>
       </c>
@@ -37481,7 +37497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="271" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:38">
       <c r="A271">
         <v>205</v>
       </c>
@@ -37597,7 +37613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="272" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:38">
       <c r="A272">
         <v>320</v>
       </c>
@@ -37713,7 +37729,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="273" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:38">
       <c r="A273">
         <v>321</v>
       </c>
@@ -37829,7 +37845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="274" spans="1:38" ht="15" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:38">
       <c r="A274">
         <v>206</v>
       </c>
@@ -37945,7 +37961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="275" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:38">
       <c r="A275">
         <v>322</v>
       </c>
@@ -38061,7 +38077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="276" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:38">
       <c r="A276">
         <v>207</v>
       </c>
@@ -38177,7 +38193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="277" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:38">
       <c r="A277">
         <v>208</v>
       </c>
@@ -38293,7 +38309,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="278" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:38">
       <c r="A278">
         <v>323</v>
       </c>
@@ -38409,7 +38425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="279" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:38">
       <c r="A279">
         <v>209</v>
       </c>
@@ -38525,7 +38541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="280" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:38">
       <c r="A280">
         <v>210</v>
       </c>
@@ -38641,7 +38657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="281" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:38">
       <c r="A281" s="6">
         <v>211</v>
       </c>
@@ -38757,7 +38773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="282" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:38">
       <c r="A282">
         <v>324</v>
       </c>
@@ -38873,7 +38889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="283" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:38">
       <c r="A283">
         <v>212</v>
       </c>
@@ -38989,7 +39005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="284" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:38">
       <c r="A284">
         <v>213</v>
       </c>
@@ -39105,7 +39121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="285" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:38">
       <c r="A285">
         <v>215</v>
       </c>
@@ -39221,7 +39237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="286" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:38">
       <c r="A286">
         <v>214</v>
       </c>
@@ -39337,7 +39353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="287" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:38">
       <c r="A287">
         <v>216</v>
       </c>
@@ -39453,7 +39469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="288" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:38">
       <c r="A288">
         <v>217</v>
       </c>
@@ -39569,7 +39585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="289" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:38">
       <c r="A289">
         <v>219</v>
       </c>
@@ -39685,7 +39701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="290" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:38">
       <c r="A290">
         <v>220</v>
       </c>
@@ -39801,7 +39817,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="291" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:38">
       <c r="A291">
         <v>221</v>
       </c>
@@ -39917,7 +39933,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="292" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:38">
       <c r="A292">
         <v>222</v>
       </c>
@@ -40033,7 +40049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="293" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:38">
       <c r="A293">
         <v>223</v>
       </c>
@@ -40149,7 +40165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="294" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:38">
       <c r="A294">
         <v>325</v>
       </c>
@@ -40265,7 +40281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="295" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:38">
       <c r="A295" s="6">
         <v>224</v>
       </c>
@@ -40381,7 +40397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="296" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:38">
       <c r="A296">
         <v>327</v>
       </c>
@@ -40497,7 +40513,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="297" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:38">
       <c r="A297">
         <v>328</v>
       </c>
@@ -40613,7 +40629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="298" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:38">
       <c r="A298">
         <v>225</v>
       </c>
@@ -40729,7 +40745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="299" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:38">
       <c r="A299" s="6">
         <v>329</v>
       </c>
@@ -40845,7 +40861,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="300" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:38">
       <c r="A300">
         <v>226</v>
       </c>
@@ -40961,7 +40977,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="301" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:38">
       <c r="A301">
         <v>330</v>
       </c>
@@ -41077,7 +41093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="302" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:38">
       <c r="A302">
         <v>229</v>
       </c>
@@ -41193,7 +41209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="303" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:38">
       <c r="A303">
         <v>230</v>
       </c>
@@ -41309,7 +41325,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="304" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:38">
       <c r="A304">
         <v>232</v>
       </c>
@@ -41425,7 +41441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="305" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:38">
       <c r="A305">
         <v>233</v>
       </c>
@@ -41541,7 +41557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="306" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:38">
       <c r="A306">
         <v>234</v>
       </c>
@@ -41657,7 +41673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="307" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:38">
       <c r="A307">
         <v>235</v>
       </c>
@@ -41773,7 +41789,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="308" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:38">
       <c r="A308">
         <v>236</v>
       </c>
@@ -41889,7 +41905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="309" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:38">
       <c r="A309">
         <v>237</v>
       </c>
@@ -42005,7 +42021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="310" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:38">
       <c r="A310">
         <v>332</v>
       </c>
@@ -42121,7 +42137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="311" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:38">
       <c r="A311">
         <v>238</v>
       </c>
@@ -42237,7 +42253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="312" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:38">
       <c r="A312">
         <v>239</v>
       </c>
@@ -42353,7 +42369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="313" spans="1:38" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:38" ht="20.399999999999999">
       <c r="A313" s="6">
         <v>240</v>
       </c>
@@ -42469,7 +42485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="314" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:38">
       <c r="A314">
         <v>242</v>
       </c>
@@ -42585,7 +42601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="315" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:38">
       <c r="A315">
         <v>243</v>
       </c>
@@ -42701,7 +42717,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="316" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:38">
       <c r="A316">
         <v>333</v>
       </c>
@@ -42817,7 +42833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="317" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:38">
       <c r="A317">
         <v>244</v>
       </c>
@@ -42933,7 +42949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="318" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:38">
       <c r="A318">
         <v>245</v>
       </c>
@@ -43049,7 +43065,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="319" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:38">
       <c r="A319">
         <v>246</v>
       </c>
@@ -43165,7 +43181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="320" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:38">
       <c r="A320">
         <v>334</v>
       </c>
@@ -43281,7 +43297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="321" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:38">
       <c r="A321">
         <v>247</v>
       </c>
@@ -43397,7 +43413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="322" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:38">
       <c r="A322">
         <v>335</v>
       </c>
@@ -43513,7 +43529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="323" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:38">
       <c r="A323">
         <v>248</v>
       </c>
@@ -43629,7 +43645,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="324" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:38">
       <c r="A324">
         <v>228</v>
       </c>
@@ -43745,7 +43761,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="325" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:38">
       <c r="A325">
         <v>15</v>
       </c>
@@ -43861,7 +43877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="326" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:38">
       <c r="A326">
         <v>249</v>
       </c>
@@ -43977,7 +43993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="327" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:38">
       <c r="A327">
         <v>336</v>
       </c>
@@ -44093,7 +44109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="328" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:38">
       <c r="A328">
         <v>337</v>
       </c>
@@ -44209,7 +44225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="329" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:38">
       <c r="A329">
         <v>123</v>
       </c>
@@ -44325,7 +44341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="330" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:38">
       <c r="A330">
         <v>185</v>
       </c>
@@ -44441,7 +44457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="331" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:38">
       <c r="A331">
         <v>186</v>
       </c>
@@ -44557,7 +44573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="332" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:38">
       <c r="A332">
         <v>241</v>
       </c>
@@ -44672,75 +44688,75 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K97" r:id="rId1"/>
-    <hyperlink ref="K103" r:id="rId2"/>
-    <hyperlink ref="G105" r:id="rId3" display="http://www.oalib.com/journal/6879/1"/>
-    <hyperlink ref="G108" r:id="rId4" display="https://link.springer.com/book/10.1007/978-1-4471-4072-6"/>
-    <hyperlink ref="K120" r:id="rId5" display="http://citeseerx.ist.psu.edu/viewdoc/summary?doi=10.1.1.101.9163; "/>
-    <hyperlink ref="G121" r:id="rId6" display="https://leitir.is/primo_library/libweb/action/dlDisplay.do?vid=GEGNIR&amp;docId=ICE01_PRIMO000599234"/>
-    <hyperlink ref="K121" r:id="rId7"/>
-    <hyperlink ref="I129" r:id="rId8" display="http://repository.unhas.ac.id/"/>
-    <hyperlink ref="K130" r:id="rId9" display="https://www.semanticscholar.org/paper/An-analysis-of-data-characteristics-that-affect-RISH-COM/10fd83b0a0ee37b2161e0e98135470c230d513b9"/>
-    <hyperlink ref="K131" r:id="rId10"/>
-    <hyperlink ref="G132" r:id="rId11" tooltip="Current Pharmacology Reports" display="https://link.springer.com/journal/40495"/>
-    <hyperlink ref="G135" r:id="rId12" tooltip="European Radiology" display="https://link.springer.com/journal/330"/>
-    <hyperlink ref="L137" r:id="rId13"/>
-    <hyperlink ref="G143" r:id="rId14" display="https://link.springer.com/conference/icics"/>
-    <hyperlink ref="G146" r:id="rId15" tooltip="Conference Website" display="http://chi2012.acm.org/"/>
-    <hyperlink ref="L146" r:id="rId16" display="https://doi.org/10.1145/2207676.2208640"/>
-    <hyperlink ref="L148" r:id="rId17"/>
-    <hyperlink ref="L160" r:id="rId18"/>
-    <hyperlink ref="J160" r:id="rId19"/>
-    <hyperlink ref="L170" r:id="rId20" display="https://doi.org/10.1177%2F1555412010364981"/>
-    <hyperlink ref="L186" r:id="rId21" display="https://doi.org/10.1109/CONIELECOMP.2012.6189918"/>
-    <hyperlink ref="K197" r:id="rId22" display="https://pdfs.semanticscholar.org/cec0/ad7b0fc2d4d6ba45c6212d36217df1ff2bf2.pdf;http://citeseerx.ist.psu.edu/viewdoc/summary?doi=10.1.1.55.9568"/>
-    <hyperlink ref="L200" r:id="rId23" tooltip="Persistent link using digital object identifier"/>
-    <hyperlink ref="G208" r:id="rId24" display="https://app.dimensions.ai/discover/publication?and_facet_journal=jour.1083795"/>
-    <hyperlink ref="K208" r:id="rId25"/>
-    <hyperlink ref="L212" r:id="rId26"/>
-    <hyperlink ref="G212" r:id="rId27" tooltip="link to all content in Journal of Medical Imaging and Health Informatics" display="https://www.ingentaconnect.com/content/asp/jmihi"/>
-    <hyperlink ref="K213" r:id="rId28"/>
-    <hyperlink ref="G213" r:id="rId29" display="https://ieeexplore.ieee.org/xpl/mostRecentIssue.jsp?punumber=6679357"/>
-    <hyperlink ref="G219" r:id="rId30" tooltip="Waste and Biomass Valorization" display="https://link.springer.com/journal/12649"/>
-    <hyperlink ref="L222" r:id="rId31" display="https://doi.org/10.1109/MCOM.2010.5673086"/>
-    <hyperlink ref="G222" r:id="rId32" display="https://ieeexplore.ieee.org/xpl/RecentIssue.jsp?punumber=35"/>
-    <hyperlink ref="L223" r:id="rId33" tooltip="Persistent link using digital object identifier"/>
-    <hyperlink ref="G228" r:id="rId34" display="https://library.seg.org/doi/book/10.1190/SEGEAB.19"/>
-    <hyperlink ref="L228" r:id="rId35" tooltip="Opens new window"/>
-    <hyperlink ref="L234" r:id="rId36"/>
-    <hyperlink ref="K237" r:id="rId37" display="http://cdn.iiit.ac.in/cdn/speech.iiit.ac.in/svlpubs/conference/Kishore2002a.pdf"/>
-    <hyperlink ref="G253" r:id="rId38" display="https://findit.dtu.dk/en/journal?ignore_search=%E2%9C%93&amp;issn%5B%5D=19422601&amp;key=19422601%7C000088%7C000004%7C000003%7C000000"/>
-    <hyperlink ref="J257" r:id="rId39"/>
-    <hyperlink ref="L258" r:id="rId40" display="https://doi.org/10.1177%2F1528083714532113"/>
-    <hyperlink ref="L269" r:id="rId41" tooltip="Persistent link using digital object identifier"/>
-    <hyperlink ref="G272" r:id="rId42" display="https://ukm.pure.elsevier.com/en/publications/heuristic-optimization-techniques-to-determine-optimal-capacitor-"/>
-    <hyperlink ref="L282" r:id="rId43"/>
-    <hyperlink ref="K283" r:id="rId44"/>
-    <hyperlink ref="L284" r:id="rId45"/>
-    <hyperlink ref="L286" r:id="rId46" display="https://doi.org/10.1109/SECON.2009.5174082"/>
-    <hyperlink ref="L291" r:id="rId47" tooltip="Persistent link using digital object identifier"/>
-    <hyperlink ref="L293" r:id="rId48" tooltip="Persistent link using digital object identifier"/>
-    <hyperlink ref="K297" r:id="rId49"/>
-    <hyperlink ref="L300" r:id="rId50" display="https://doi.org/10.1109/NUICONE.2015.7449639"/>
-    <hyperlink ref="G300" r:id="rId51" display="https://ieeexplore.ieee.org/xpl/mostRecentIssue.jsp?punumber=7446021"/>
-    <hyperlink ref="L301" r:id="rId52" display="https://doi.org/10.1109/IECON.2013.6699111"/>
-    <hyperlink ref="G302" r:id="rId53" tooltip="Conference Website" display="https://www.acm.org/conferences/sac/sac2015/"/>
-    <hyperlink ref="L302" r:id="rId54" display="https://doi.org/10.1145/2695664.2695719"/>
-    <hyperlink ref="L304" r:id="rId55" tooltip="Persistent link using digital object identifier"/>
-    <hyperlink ref="G307" r:id="rId56" display="http://journaldatabase.info/journal/issn2229-6093"/>
-    <hyperlink ref="L311" r:id="rId57" display="https://doi.org/10.1109/WHISPERS.2014.8077520"/>
-    <hyperlink ref="L312" r:id="rId58" display="https://dx.doi.org/10.1016%2Fj.trstmh.2010.09.007"/>
-    <hyperlink ref="L316" r:id="rId59" tooltip="Persistent link using digital object identifier"/>
-    <hyperlink ref="L318" r:id="rId60" tooltip="Persistent link using digital object identifier"/>
-    <hyperlink ref="G320" r:id="rId61" display="https://www.igi-global.com/book/big-data-management-technologies-applications/77404"/>
-    <hyperlink ref="G321" r:id="rId62" display="https://link.springer.com/referencework/10.1007/978-94-007-6064-6"/>
-    <hyperlink ref="G322" r:id="rId63" display="https://ieeexplore.ieee.org/xpl/mostRecentIssue.jsp?punumber=9626"/>
-    <hyperlink ref="L322" r:id="rId64" display="https://doi.org/10.1109/ACSSC.2004.1399438"/>
-    <hyperlink ref="J323" r:id="rId65"/>
-    <hyperlink ref="L326" r:id="rId66" display="https://doi.org/10.1145/2030112.2030127"/>
-    <hyperlink ref="K255" r:id="rId67"/>
-    <hyperlink ref="J299" r:id="rId68"/>
-    <hyperlink ref="K299" r:id="rId69"/>
+    <hyperlink ref="K97" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="K103" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="G105" r:id="rId3" display="http://www.oalib.com/journal/6879/1" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="G108" r:id="rId4" display="https://link.springer.com/book/10.1007/978-1-4471-4072-6" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="K120" r:id="rId5" display="http://citeseerx.ist.psu.edu/viewdoc/summary?doi=10.1.1.101.9163; " xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="G121" r:id="rId6" display="https://leitir.is/primo_library/libweb/action/dlDisplay.do?vid=GEGNIR&amp;docId=ICE01_PRIMO000599234" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="K121" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="I129" r:id="rId8" display="http://repository.unhas.ac.id/" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="K130" r:id="rId9" display="https://www.semanticscholar.org/paper/An-analysis-of-data-characteristics-that-affect-RISH-COM/10fd83b0a0ee37b2161e0e98135470c230d513b9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="K131" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="G132" r:id="rId11" tooltip="Current Pharmacology Reports" display="https://link.springer.com/journal/40495" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="G135" r:id="rId12" tooltip="European Radiology" display="https://link.springer.com/journal/330" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="L137" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="G143" r:id="rId14" display="https://link.springer.com/conference/icics" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="G146" r:id="rId15" tooltip="Conference Website" display="http://chi2012.acm.org/" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="L146" r:id="rId16" display="https://doi.org/10.1145/2207676.2208640" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="L148" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="L160" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="J160" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="L170" r:id="rId20" display="https://doi.org/10.1177%2F1555412010364981" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="L186" r:id="rId21" display="https://doi.org/10.1109/CONIELECOMP.2012.6189918" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="K197" r:id="rId22" display="https://pdfs.semanticscholar.org/cec0/ad7b0fc2d4d6ba45c6212d36217df1ff2bf2.pdf;http://citeseerx.ist.psu.edu/viewdoc/summary?doi=10.1.1.55.9568" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="L200" r:id="rId23" tooltip="Persistent link using digital object identifier" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="G208" r:id="rId24" display="https://app.dimensions.ai/discover/publication?and_facet_journal=jour.1083795" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="K208" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="L212" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="G212" r:id="rId27" tooltip="link to all content in Journal of Medical Imaging and Health Informatics" display="https://www.ingentaconnect.com/content/asp/jmihi" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="K213" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="G213" r:id="rId29" display="https://ieeexplore.ieee.org/xpl/mostRecentIssue.jsp?punumber=6679357" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="G219" r:id="rId30" tooltip="Waste and Biomass Valorization" display="https://link.springer.com/journal/12649" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="L222" r:id="rId31" display="https://doi.org/10.1109/MCOM.2010.5673086" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="G222" r:id="rId32" display="https://ieeexplore.ieee.org/xpl/RecentIssue.jsp?punumber=35" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="L223" r:id="rId33" tooltip="Persistent link using digital object identifier" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="G228" r:id="rId34" display="https://library.seg.org/doi/book/10.1190/SEGEAB.19" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="L228" r:id="rId35" tooltip="Opens new window" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="L234" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="K237" r:id="rId37" display="http://cdn.iiit.ac.in/cdn/speech.iiit.ac.in/svlpubs/conference/Kishore2002a.pdf" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="G253" r:id="rId38" display="https://findit.dtu.dk/en/journal?ignore_search=%E2%9C%93&amp;issn%5B%5D=19422601&amp;key=19422601%7C000088%7C000004%7C000003%7C000000" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="J257" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="L258" r:id="rId40" display="https://doi.org/10.1177%2F1528083714532113" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="L269" r:id="rId41" tooltip="Persistent link using digital object identifier" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="G272" r:id="rId42" display="https://ukm.pure.elsevier.com/en/publications/heuristic-optimization-techniques-to-determine-optimal-capacitor-" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="L282" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="K283" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="L284" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="L286" r:id="rId46" display="https://doi.org/10.1109/SECON.2009.5174082" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="L291" r:id="rId47" tooltip="Persistent link using digital object identifier" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="L293" r:id="rId48" tooltip="Persistent link using digital object identifier" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="K297" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="L300" r:id="rId50" display="https://doi.org/10.1109/NUICONE.2015.7449639" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="G300" r:id="rId51" display="https://ieeexplore.ieee.org/xpl/mostRecentIssue.jsp?punumber=7446021" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="L301" r:id="rId52" display="https://doi.org/10.1109/IECON.2013.6699111" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="G302" r:id="rId53" tooltip="Conference Website" display="https://www.acm.org/conferences/sac/sac2015/" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="L302" r:id="rId54" display="https://doi.org/10.1145/2695664.2695719" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="L304" r:id="rId55" tooltip="Persistent link using digital object identifier" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="G307" r:id="rId56" display="http://journaldatabase.info/journal/issn2229-6093" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="L311" r:id="rId57" display="https://doi.org/10.1109/WHISPERS.2014.8077520" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="L312" r:id="rId58" display="https://dx.doi.org/10.1016%2Fj.trstmh.2010.09.007" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="L316" r:id="rId59" tooltip="Persistent link using digital object identifier" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="L318" r:id="rId60" tooltip="Persistent link using digital object identifier" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="G320" r:id="rId61" display="https://www.igi-global.com/book/big-data-management-technologies-applications/77404" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="G321" r:id="rId62" display="https://link.springer.com/referencework/10.1007/978-94-007-6064-6" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="G322" r:id="rId63" display="https://ieeexplore.ieee.org/xpl/mostRecentIssue.jsp?punumber=9626" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="L322" r:id="rId64" display="https://doi.org/10.1109/ACSSC.2004.1399438" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="J323" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="L326" r:id="rId66" display="https://doi.org/10.1145/2030112.2030127" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="K255" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="J299" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="K299" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId70"/>

</xml_diff>

<commit_message>
Update after checking consistancy
</commit_message>
<xml_diff>
--- a/ProcessedData/WOS_SciConf_20180531_YeEdited20181113.xlsx
+++ b/ProcessedData/WOS_SciConf_20180531_YeEdited20181113.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\adit\My Documents\RG Citations\rgciting\ProcessedData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\adit\Desktop\citing\citation\rgciting\ProcessedData\Modified Excel Workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15E23F07-1DD7-43B3-8E81-21F29F24208F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9600" windowHeight="3312" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9600" windowHeight="3315"/>
   </bookViews>
   <sheets>
     <sheet name="WOS_SciConf_20180531 (R1)" sheetId="1" r:id="rId1"/>
@@ -23,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11235" uniqueCount="1737">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11235" uniqueCount="1747">
   <si>
     <t>AID</t>
   </si>
@@ -5242,13 +5241,43 @@
   </si>
   <si>
     <t>https://zdoc.site/history-and-applications-of-hydrogels-journal-of-biomedical-.html</t>
+  </si>
+  <si>
+    <t>Analytical Letters</t>
+  </si>
+  <si>
+    <t>10.1080/00032719.2012.677779</t>
+  </si>
+  <si>
+    <t>Agriculturae Conspectus Scientificus</t>
+  </si>
+  <si>
+    <t>https://acs.agr.hr/acs/index.php/acs/article/view/68; ttps://www.academia.edu/1009136/Antioxidant_activity_and_polyphenols_of_Aronia_in_comparison_to_other_berry_species; https://www.semanticscholar.org/paper/Antioxidant-Activity-and-Polyphenols-of-Aronia-in-Jakobek/b5a2cd69aca19e5f3efae06f5b10497b8585a47e</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/ftp/arxiv/papers/0704/0704.2862.pdf</t>
+  </si>
+  <si>
+    <t>Nanotechnology</t>
+  </si>
+  <si>
+    <t>10.1088/0957-4484/18/46/465202</t>
+  </si>
+  <si>
+    <t>cienciared.com</t>
+  </si>
+  <si>
+    <t>fisec-estrategias</t>
+  </si>
+  <si>
+    <t>http://www.cienciared.com.ar/ra/doc.php?n=1362; http://www.cienciared.com.ar/ra/usr/9/313/fisec_estrategias_n14m3pp37_55.pdf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="26">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -6167,32 +6196,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL332"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A314" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="L61" sqref="L61"/>
+      <selection pane="bottomLeft" activeCell="A325" sqref="A325"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="21.5546875" customWidth="1"/>
+    <col min="7" max="7" width="21.5703125" customWidth="1"/>
     <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="35.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="60.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="255.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.33203125" customWidth="1"/>
-    <col min="13" max="13" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.5703125" customWidth="1"/>
+    <col min="11" max="11" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" customWidth="1"/>
+    <col min="13" max="13" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="31" customWidth="1"/>
-    <col min="20" max="20" width="7.33203125" customWidth="1"/>
-    <col min="21" max="21" width="7.77734375" customWidth="1"/>
-    <col min="22" max="22" width="31.6640625" customWidth="1"/>
+    <col min="20" max="20" width="7.28515625" customWidth="1"/>
+    <col min="21" max="21" width="7.7109375" customWidth="1"/>
+    <col min="22" max="22" width="31.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -6305,7 +6334,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:38">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>183</v>
       </c>
@@ -6421,7 +6450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:38">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>184</v>
       </c>
@@ -6537,7 +6566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:38">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>187</v>
       </c>
@@ -6653,7 +6682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:38">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>227</v>
       </c>
@@ -6769,7 +6798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:38">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>250</v>
       </c>
@@ -6885,7 +6914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:38">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>338</v>
       </c>
@@ -7001,7 +7030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:38">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -7117,7 +7146,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:38">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>251</v>
       </c>
@@ -7233,7 +7262,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:38">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2</v>
       </c>
@@ -7349,7 +7378,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:38">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>3</v>
       </c>
@@ -7465,7 +7494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:38">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>4</v>
       </c>
@@ -7581,7 +7610,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:38">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>5</v>
       </c>
@@ -7697,7 +7726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:38">
+    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>6</v>
       </c>
@@ -7813,7 +7842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:38">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>7</v>
       </c>
@@ -7929,7 +7958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:38">
+    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>253</v>
       </c>
@@ -8045,123 +8074,123 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:38">
-      <c r="A17">
+    <row r="17" spans="1:38" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
         <v>9</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="C17" t="s">
-        <v>45</v>
-      </c>
-      <c r="D17" t="s">
-        <v>45</v>
-      </c>
-      <c r="E17" t="s">
-        <v>45</v>
-      </c>
-      <c r="F17" t="s">
-        <v>45</v>
-      </c>
-      <c r="G17" t="s">
-        <v>45</v>
-      </c>
-      <c r="H17" t="s">
-        <v>45</v>
-      </c>
-      <c r="I17" t="s">
-        <v>45</v>
-      </c>
-      <c r="J17" t="s">
-        <v>45</v>
-      </c>
-      <c r="K17" t="s">
-        <v>45</v>
-      </c>
-      <c r="L17" t="s">
-        <v>45</v>
-      </c>
-      <c r="M17" t="s">
-        <v>45</v>
-      </c>
-      <c r="N17" t="s">
-        <v>45</v>
-      </c>
-      <c r="O17" t="s">
-        <v>45</v>
-      </c>
-      <c r="P17" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q17" t="s">
+      <c r="C17" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>1721</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="L17" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="M17" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="N17" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="O17" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="P17" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q17" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="R17" t="s">
+      <c r="R17" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="S17" t="s">
-        <v>45</v>
-      </c>
-      <c r="T17" t="s">
-        <v>45</v>
-      </c>
-      <c r="U17" t="s">
-        <v>45</v>
-      </c>
-      <c r="V17" t="s">
-        <v>45</v>
-      </c>
-      <c r="W17" t="s">
-        <v>45</v>
-      </c>
-      <c r="X17" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y17" t="s">
+      <c r="S17" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="T17" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="U17" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="V17" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="W17" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="X17" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y17" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="Z17">
+      <c r="Z17" s="6">
         <v>3</v>
       </c>
-      <c r="AA17" t="s">
-        <v>45</v>
-      </c>
-      <c r="AB17" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC17" t="s">
-        <v>45</v>
-      </c>
-      <c r="AD17" t="s">
-        <v>45</v>
-      </c>
-      <c r="AE17" t="s">
-        <v>45</v>
-      </c>
-      <c r="AF17" t="s">
+      <c r="AA17" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB17" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC17" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="AD17" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="AE17" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF17" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="AG17">
+      <c r="AG17" s="6">
         <v>1980</v>
       </c>
-      <c r="AH17" t="s">
-        <v>45</v>
-      </c>
-      <c r="AI17" t="s">
-        <v>45</v>
-      </c>
-      <c r="AJ17" t="s">
-        <v>45</v>
-      </c>
-      <c r="AK17" t="s">
-        <v>45</v>
-      </c>
-      <c r="AL17">
+      <c r="AH17" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="AI17" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="AJ17" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK17" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="AL17" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:38">
+    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>10</v>
       </c>
@@ -8277,7 +8306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:38">
+    <row r="19" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>11</v>
       </c>
@@ -8393,7 +8422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:38">
+    <row r="20" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>12</v>
       </c>
@@ -8509,7 +8538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:38">
+    <row r="21" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>13</v>
       </c>
@@ -8625,7 +8654,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:38">
+    <row r="22" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>14</v>
       </c>
@@ -8741,7 +8770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:38">
+    <row r="23" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>16</v>
       </c>
@@ -8857,7 +8886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:38">
+    <row r="24" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>17</v>
       </c>
@@ -8973,7 +9002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:38">
+    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>254</v>
       </c>
@@ -9089,7 +9118,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:38">
+    <row r="26" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>18</v>
       </c>
@@ -9205,7 +9234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:38">
+    <row r="27" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>19</v>
       </c>
@@ -9321,7 +9350,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:38">
+    <row r="28" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>20</v>
       </c>
@@ -9437,7 +9466,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:38">
+    <row r="29" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>21</v>
       </c>
@@ -9553,7 +9582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:38">
+    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>255</v>
       </c>
@@ -9669,7 +9698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:38">
+    <row r="31" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>22</v>
       </c>
@@ -9785,7 +9814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:38">
+    <row r="32" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>23</v>
       </c>
@@ -9901,7 +9930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:38">
+    <row r="33" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>24</v>
       </c>
@@ -10017,7 +10046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:38">
+    <row r="34" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>25</v>
       </c>
@@ -10133,7 +10162,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:38">
+    <row r="35" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>26</v>
       </c>
@@ -10249,7 +10278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:38">
+    <row r="36" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>27</v>
       </c>
@@ -10365,7 +10394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:38">
+    <row r="37" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>28</v>
       </c>
@@ -10481,7 +10510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:38">
+    <row r="38" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>29</v>
       </c>
@@ -10597,7 +10626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:38">
+    <row r="39" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>30</v>
       </c>
@@ -10713,7 +10742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:38">
+    <row r="40" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>31</v>
       </c>
@@ -10829,7 +10858,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:38">
+    <row r="41" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>32</v>
       </c>
@@ -10945,7 +10974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:38">
+    <row r="42" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>231</v>
       </c>
@@ -11061,7 +11090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:38">
+    <row r="43" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>33</v>
       </c>
@@ -11177,7 +11206,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:38">
+    <row r="44" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>34</v>
       </c>
@@ -11293,7 +11322,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:38">
+    <row r="45" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>256</v>
       </c>
@@ -11409,7 +11438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:38">
+    <row r="46" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>257</v>
       </c>
@@ -11525,7 +11554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:38">
+    <row r="47" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>258</v>
       </c>
@@ -11641,7 +11670,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:38">
+    <row r="48" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>259</v>
       </c>
@@ -11757,7 +11786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:38">
+    <row r="49" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>35</v>
       </c>
@@ -11873,7 +11902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:38">
+    <row r="50" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>36</v>
       </c>
@@ -11989,7 +12018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:38">
+    <row r="51" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>37</v>
       </c>
@@ -12105,7 +12134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:38">
+    <row r="52" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>260</v>
       </c>
@@ -12221,7 +12250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:38">
+    <row r="53" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>38</v>
       </c>
@@ -12337,7 +12366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:38">
+    <row r="54" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>39</v>
       </c>
@@ -12453,7 +12482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:38">
+    <row r="55" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>40</v>
       </c>
@@ -12569,7 +12598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:38">
+    <row r="56" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>41</v>
       </c>
@@ -12685,7 +12714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:38">
+    <row r="57" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>42</v>
       </c>
@@ -12801,7 +12830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:38">
+    <row r="58" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>261</v>
       </c>
@@ -12917,7 +12946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:38">
+    <row r="59" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>43</v>
       </c>
@@ -13033,7 +13062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:38">
+    <row r="60" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>44</v>
       </c>
@@ -13149,7 +13178,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:38">
+    <row r="61" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>45</v>
       </c>
@@ -13265,7 +13294,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:38">
+    <row r="62" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>46</v>
       </c>
@@ -13381,7 +13410,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:38">
+    <row r="63" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>47</v>
       </c>
@@ -13497,7 +13526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:38">
+    <row r="64" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>263</v>
       </c>
@@ -13613,7 +13642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:38">
+    <row r="65" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>48</v>
       </c>
@@ -13729,7 +13758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:38">
+    <row r="66" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>49</v>
       </c>
@@ -13845,239 +13874,239 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:38">
-      <c r="A67">
+    <row r="67" spans="1:38" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="6">
         <v>50</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="6" t="s">
         <v>395</v>
       </c>
-      <c r="C67" t="s">
-        <v>39</v>
-      </c>
-      <c r="D67" t="s">
-        <v>39</v>
-      </c>
-      <c r="E67" t="s">
-        <v>39</v>
-      </c>
-      <c r="F67" t="s">
-        <v>39</v>
-      </c>
-      <c r="G67" t="s">
+      <c r="C67" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E67" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F67" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G67" s="6" t="s">
         <v>396</v>
       </c>
-      <c r="H67" t="s">
-        <v>45</v>
-      </c>
-      <c r="I67" t="s">
-        <v>45</v>
-      </c>
-      <c r="J67" t="s">
+      <c r="H67" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I67" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="J67" s="6" t="s">
         <v>397</v>
       </c>
-      <c r="K67" t="s">
+      <c r="K67" s="6" t="s">
         <v>398</v>
       </c>
-      <c r="L67" t="s">
-        <v>45</v>
-      </c>
-      <c r="M67" t="s">
-        <v>45</v>
-      </c>
-      <c r="N67" t="s">
-        <v>45</v>
-      </c>
-      <c r="O67" t="s">
-        <v>45</v>
-      </c>
-      <c r="P67" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q67" t="s">
+      <c r="L67" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="M67" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="N67" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="O67" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="P67" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q67" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="R67" t="s">
+      <c r="R67" s="6" t="s">
         <v>399</v>
       </c>
-      <c r="S67" t="s">
-        <v>45</v>
-      </c>
-      <c r="T67" t="s">
-        <v>45</v>
-      </c>
-      <c r="U67" t="s">
-        <v>45</v>
-      </c>
-      <c r="V67" t="s">
+      <c r="S67" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="T67" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="U67" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="V67" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="W67" t="s">
-        <v>45</v>
-      </c>
-      <c r="X67" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y67" t="s">
+      <c r="W67" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="X67" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y67" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="Z67" t="s">
-        <v>45</v>
-      </c>
-      <c r="AA67" t="s">
-        <v>45</v>
-      </c>
-      <c r="AB67" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC67" t="s">
-        <v>45</v>
-      </c>
-      <c r="AD67" t="s">
-        <v>45</v>
-      </c>
-      <c r="AE67" t="s">
-        <v>45</v>
-      </c>
-      <c r="AF67" t="s">
-        <v>45</v>
-      </c>
-      <c r="AG67" t="s">
-        <v>45</v>
-      </c>
-      <c r="AH67" t="s">
-        <v>45</v>
-      </c>
-      <c r="AI67" t="s">
-        <v>45</v>
-      </c>
-      <c r="AJ67" t="s">
-        <v>45</v>
-      </c>
-      <c r="AK67" t="s">
-        <v>45</v>
-      </c>
-      <c r="AL67">
+      <c r="Z67" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA67" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB67" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC67" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="AD67" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="AE67" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF67" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="AG67" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="AH67" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="AI67" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="AJ67" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK67" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="AL67" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:38">
-      <c r="A68">
+    <row r="68" spans="1:38" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="6">
         <v>264</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="6" t="s">
         <v>401</v>
       </c>
-      <c r="C68" t="s">
-        <v>45</v>
-      </c>
-      <c r="D68" t="s">
-        <v>45</v>
-      </c>
-      <c r="E68" t="s">
-        <v>45</v>
-      </c>
-      <c r="F68" t="s">
-        <v>45</v>
-      </c>
-      <c r="G68" t="s">
-        <v>45</v>
-      </c>
-      <c r="H68" t="s">
-        <v>45</v>
-      </c>
-      <c r="I68" t="s">
-        <v>45</v>
-      </c>
-      <c r="J68" t="s">
-        <v>45</v>
-      </c>
-      <c r="K68" t="s">
-        <v>45</v>
-      </c>
-      <c r="L68" t="s">
-        <v>45</v>
-      </c>
-      <c r="M68" t="s">
-        <v>45</v>
-      </c>
-      <c r="N68" t="s">
-        <v>45</v>
-      </c>
-      <c r="O68" t="s">
-        <v>45</v>
-      </c>
-      <c r="P68" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q68" t="s">
+      <c r="C68" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D68" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E68" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F68" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G68" s="6" t="s">
+        <v>1737</v>
+      </c>
+      <c r="H68" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="I68" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="J68" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="K68" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="L68" s="6" t="s">
+        <v>1738</v>
+      </c>
+      <c r="M68" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="N68" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="O68" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="P68" s="6" t="s">
+        <v>456</v>
+      </c>
+      <c r="Q68" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="R68" t="s">
+      <c r="R68" s="6" t="s">
         <v>402</v>
       </c>
-      <c r="S68" t="s">
-        <v>45</v>
-      </c>
-      <c r="T68" t="s">
-        <v>45</v>
-      </c>
-      <c r="U68" t="s">
-        <v>45</v>
-      </c>
-      <c r="V68" t="s">
-        <v>45</v>
-      </c>
-      <c r="W68" t="s">
-        <v>45</v>
-      </c>
-      <c r="X68" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y68" t="s">
+      <c r="S68" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="T68" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="U68" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="V68" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="W68" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="X68" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y68" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="Z68">
+      <c r="Z68" s="6">
         <v>4</v>
       </c>
-      <c r="AA68" t="s">
-        <v>45</v>
-      </c>
-      <c r="AB68">
+      <c r="AA68" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB68" s="6">
         <v>1557</v>
       </c>
-      <c r="AC68">
+      <c r="AC68" s="6">
         <v>1565</v>
       </c>
-      <c r="AD68" t="s">
-        <v>45</v>
-      </c>
-      <c r="AE68" t="s">
-        <v>45</v>
-      </c>
-      <c r="AF68" t="s">
-        <v>45</v>
-      </c>
-      <c r="AG68">
+      <c r="AD68" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="AE68" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF68" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="AG68" s="6">
         <v>2013</v>
       </c>
-      <c r="AH68" t="s">
-        <v>45</v>
-      </c>
-      <c r="AI68" t="s">
-        <v>45</v>
-      </c>
-      <c r="AJ68" t="s">
-        <v>45</v>
-      </c>
-      <c r="AK68" t="s">
-        <v>45</v>
-      </c>
-      <c r="AL68">
+      <c r="AH68" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="AI68" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="AJ68" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK68" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="AL68" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:38">
+    <row r="69" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>265</v>
       </c>
@@ -14193,7 +14222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:38">
+    <row r="70" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>51</v>
       </c>
@@ -14309,7 +14338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:38">
+    <row r="71" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>266</v>
       </c>
@@ -14425,7 +14454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:38">
+    <row r="72" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>54</v>
       </c>
@@ -14541,7 +14570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:38">
+    <row r="73" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>52</v>
       </c>
@@ -14657,7 +14686,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="1:38">
+    <row r="74" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>317</v>
       </c>
@@ -14773,7 +14802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:38">
+    <row r="75" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>53</v>
       </c>
@@ -14889,7 +14918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:38">
+    <row r="76" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>56</v>
       </c>
@@ -15005,7 +15034,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="1:38">
+    <row r="77" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>57</v>
       </c>
@@ -15121,7 +15150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:38">
+    <row r="78" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>58</v>
       </c>
@@ -15237,7 +15266,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="79" spans="1:38">
+    <row r="79" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>267</v>
       </c>
@@ -15353,7 +15382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:38">
+    <row r="80" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>59</v>
       </c>
@@ -15469,7 +15498,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:38">
+    <row r="81" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>60</v>
       </c>
@@ -15585,7 +15614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:38">
+    <row r="82" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>61</v>
       </c>
@@ -15701,7 +15730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:38">
+    <row r="83" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>55</v>
       </c>
@@ -15817,7 +15846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:38">
+    <row r="84" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>268</v>
       </c>
@@ -15933,7 +15962,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="85" spans="1:38">
+    <row r="85" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>269</v>
       </c>
@@ -16049,7 +16078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:38">
+    <row r="86" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>62</v>
       </c>
@@ -16165,7 +16194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:38">
+    <row r="87" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>270</v>
       </c>
@@ -16281,7 +16310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:38">
+    <row r="88" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>63</v>
       </c>
@@ -16397,7 +16426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:38">
+    <row r="89" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>64</v>
       </c>
@@ -16513,7 +16542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:38">
+    <row r="90" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>271</v>
       </c>
@@ -16629,7 +16658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:38">
+    <row r="91" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>65</v>
       </c>
@@ -16745,7 +16774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:38">
+    <row r="92" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>66</v>
       </c>
@@ -16861,7 +16890,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:38">
+    <row r="93" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>195</v>
       </c>
@@ -16977,7 +17006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:38">
+    <row r="94" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>67</v>
       </c>
@@ -17093,7 +17122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:38">
+    <row r="95" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>68</v>
       </c>
@@ -17209,7 +17238,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:38">
+    <row r="96" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>69</v>
       </c>
@@ -17325,7 +17354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:38">
+    <row r="97" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>70</v>
       </c>
@@ -17441,7 +17470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:38">
+    <row r="98" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>71</v>
       </c>
@@ -17557,7 +17586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:38">
+    <row r="99" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>72</v>
       </c>
@@ -17673,7 +17702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:38">
+    <row r="100" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>73</v>
       </c>
@@ -17789,7 +17818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:38">
+    <row r="101" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>272</v>
       </c>
@@ -17905,7 +17934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:38">
+    <row r="102" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>74</v>
       </c>
@@ -18021,7 +18050,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="103" spans="1:38">
+    <row r="103" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>75</v>
       </c>
@@ -18137,7 +18166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:38" ht="15">
+    <row r="104" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>76</v>
       </c>
@@ -18253,7 +18282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:38">
+    <row r="105" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>77</v>
       </c>
@@ -18369,7 +18398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:38">
+    <row r="106" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>78</v>
       </c>
@@ -18485,7 +18514,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:38">
+    <row r="107" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>79</v>
       </c>
@@ -18601,7 +18630,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="108" spans="1:38">
+    <row r="108" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>80</v>
       </c>
@@ -18717,7 +18746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:38">
+    <row r="109" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A109" s="6">
         <v>81</v>
       </c>
@@ -18833,7 +18862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:38">
+    <row r="110" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>82</v>
       </c>
@@ -18949,7 +18978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:38">
+    <row r="111" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>83</v>
       </c>
@@ -19065,7 +19094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:38">
+    <row r="112" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>273</v>
       </c>
@@ -19181,7 +19210,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:38">
+    <row r="113" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>84</v>
       </c>
@@ -19297,7 +19326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:38">
+    <row r="114" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>85</v>
       </c>
@@ -19413,7 +19442,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:38">
+    <row r="115" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>86</v>
       </c>
@@ -19529,7 +19558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:38">
+    <row r="116" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>87</v>
       </c>
@@ -19645,7 +19674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:38">
+    <row r="117" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>88</v>
       </c>
@@ -19761,7 +19790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:38">
+    <row r="118" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>89</v>
       </c>
@@ -19877,7 +19906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:38">
+    <row r="119" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>90</v>
       </c>
@@ -19993,7 +20022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:38">
+    <row r="120" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>91</v>
       </c>
@@ -20109,7 +20138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:38">
+    <row r="121" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>92</v>
       </c>
@@ -20225,7 +20254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:38">
+    <row r="122" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>93</v>
       </c>
@@ -20341,7 +20370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:38">
+    <row r="123" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>94</v>
       </c>
@@ -20454,7 +20483,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="124" spans="1:38">
+    <row r="124" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>95</v>
       </c>
@@ -20570,7 +20599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:38">
+    <row r="125" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>126</v>
       </c>
@@ -20686,7 +20715,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="126" spans="1:38">
+    <row r="126" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>96</v>
       </c>
@@ -20802,7 +20831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:38">
+    <row r="127" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>97</v>
       </c>
@@ -20918,7 +20947,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:38">
+    <row r="128" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>98</v>
       </c>
@@ -21034,7 +21063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:38">
+    <row r="129" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>99</v>
       </c>
@@ -21150,7 +21179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:38">
+    <row r="130" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>100</v>
       </c>
@@ -21266,7 +21295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:38">
+    <row r="131" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>101</v>
       </c>
@@ -21382,7 +21411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:38">
+    <row r="132" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>102</v>
       </c>
@@ -21498,7 +21527,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:38">
+    <row r="133" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>103</v>
       </c>
@@ -21614,7 +21643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:38">
+    <row r="134" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>104</v>
       </c>
@@ -21622,43 +21651,43 @@
         <v>682</v>
       </c>
       <c r="C134" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D134" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E134" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="F134" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="G134" t="s">
-        <v>45</v>
+        <v>1739</v>
       </c>
       <c r="H134" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="I134" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="J134" t="s">
-        <v>45</v>
+        <v>121</v>
       </c>
       <c r="K134" t="s">
-        <v>45</v>
+        <v>1740</v>
       </c>
       <c r="L134" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="M134" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="N134" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="O134" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="P134" t="s">
         <v>45</v>
@@ -21730,7 +21759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:38">
+    <row r="135" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>275</v>
       </c>
@@ -21846,7 +21875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:38">
+    <row r="136" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>105</v>
       </c>
@@ -21962,7 +21991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:38">
+    <row r="137" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>106</v>
       </c>
@@ -22078,7 +22107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:38">
+    <row r="138" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>276</v>
       </c>
@@ -22194,7 +22223,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:38">
+    <row r="139" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>107</v>
       </c>
@@ -22310,7 +22339,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:38">
+    <row r="140" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>108</v>
       </c>
@@ -22426,7 +22455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:38">
+    <row r="141" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>277</v>
       </c>
@@ -22542,7 +22571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:38">
+    <row r="142" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>109</v>
       </c>
@@ -22658,7 +22687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:38">
+    <row r="143" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>110</v>
       </c>
@@ -22774,7 +22803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:38">
+    <row r="144" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>111</v>
       </c>
@@ -22890,7 +22919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:38">
+    <row r="145" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>112</v>
       </c>
@@ -22898,46 +22927,46 @@
         <v>717</v>
       </c>
       <c r="C145" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D145" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E145" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="F145" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="G145" t="s">
-        <v>45</v>
+        <v>1742</v>
       </c>
       <c r="H145" t="s">
-        <v>45</v>
+        <v>1365</v>
       </c>
       <c r="I145" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="J145" t="s">
-        <v>45</v>
-      </c>
-      <c r="K145" t="s">
-        <v>45</v>
+        <v>39</v>
+      </c>
+      <c r="K145" s="3" t="s">
+        <v>1741</v>
       </c>
       <c r="L145" t="s">
-        <v>45</v>
+        <v>1743</v>
       </c>
       <c r="M145" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="N145" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="O145" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="P145" t="s">
-        <v>45</v>
+        <v>456</v>
       </c>
       <c r="Q145" t="s">
         <v>43</v>
@@ -23006,7 +23035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:38">
+    <row r="146" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>278</v>
       </c>
@@ -23122,7 +23151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:38">
+    <row r="147" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>113</v>
       </c>
@@ -23238,7 +23267,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:38">
+    <row r="148" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>114</v>
       </c>
@@ -23354,7 +23383,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:38">
+    <row r="149" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>115</v>
       </c>
@@ -23470,7 +23499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:38">
+    <row r="150" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>116</v>
       </c>
@@ -23586,7 +23615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:38">
+    <row r="151" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>117</v>
       </c>
@@ -23702,7 +23731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:38">
+    <row r="152" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>118</v>
       </c>
@@ -23818,7 +23847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:38">
+    <row r="153" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>279</v>
       </c>
@@ -23934,7 +23963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:38">
+    <row r="154" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>119</v>
       </c>
@@ -24050,7 +24079,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:38">
+    <row r="155" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>120</v>
       </c>
@@ -24166,7 +24195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:38">
+    <row r="156" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>280</v>
       </c>
@@ -24282,7 +24311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:38">
+    <row r="157" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>281</v>
       </c>
@@ -24398,7 +24427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:38">
+    <row r="158" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>121</v>
       </c>
@@ -24514,7 +24543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:38">
+    <row r="159" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>282</v>
       </c>
@@ -24630,7 +24659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:38">
+    <row r="160" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>122</v>
       </c>
@@ -24746,7 +24775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:38">
+    <row r="161" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>128</v>
       </c>
@@ -24862,7 +24891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:38">
+    <row r="162" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>124</v>
       </c>
@@ -24978,7 +25007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:38">
+    <row r="163" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>125</v>
       </c>
@@ -25094,7 +25123,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:38">
+    <row r="164" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>127</v>
       </c>
@@ -25210,7 +25239,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:38">
+    <row r="165" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>283</v>
       </c>
@@ -25326,7 +25355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:38">
+    <row r="166" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>284</v>
       </c>
@@ -25442,7 +25471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:38">
+    <row r="167" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>129</v>
       </c>
@@ -25558,7 +25587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:38">
+    <row r="168" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>130</v>
       </c>
@@ -25674,7 +25703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:38">
+    <row r="169" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>131</v>
       </c>
@@ -25790,7 +25819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:38">
+    <row r="170" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>132</v>
       </c>
@@ -25906,7 +25935,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:38">
+    <row r="171" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>285</v>
       </c>
@@ -26022,7 +26051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:38">
+    <row r="172" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>133</v>
       </c>
@@ -26138,7 +26167,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:38">
+    <row r="173" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>134</v>
       </c>
@@ -26254,7 +26283,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:38">
+    <row r="174" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>135</v>
       </c>
@@ -26370,7 +26399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:38">
+    <row r="175" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>136</v>
       </c>
@@ -26486,7 +26515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:38">
+    <row r="176" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>286</v>
       </c>
@@ -26602,7 +26631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:38">
+    <row r="177" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>138</v>
       </c>
@@ -26718,7 +26747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:38">
+    <row r="178" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>137</v>
       </c>
@@ -26834,7 +26863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:38">
+    <row r="179" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>139</v>
       </c>
@@ -26950,7 +26979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:38">
+    <row r="180" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A180" s="6">
         <v>218</v>
       </c>
@@ -27066,7 +27095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:38">
+    <row r="181" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>287</v>
       </c>
@@ -27182,7 +27211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:38">
+    <row r="182" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>140</v>
       </c>
@@ -27298,7 +27327,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:38">
+    <row r="183" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>141</v>
       </c>
@@ -27414,7 +27443,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="184" spans="1:38">
+    <row r="184" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>142</v>
       </c>
@@ -27530,7 +27559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:38">
+    <row r="185" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>143</v>
       </c>
@@ -27538,43 +27567,43 @@
         <v>837</v>
       </c>
       <c r="C185" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D185" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E185" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="F185" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="G185" t="s">
-        <v>45</v>
+        <v>1745</v>
       </c>
       <c r="H185" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="I185" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="J185" t="s">
-        <v>45</v>
+        <v>1744</v>
       </c>
       <c r="K185" t="s">
-        <v>45</v>
+        <v>1746</v>
       </c>
       <c r="L185" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="M185" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="N185" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="O185" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="P185" t="s">
         <v>45</v>
@@ -27646,7 +27675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:38">
+    <row r="186" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>288</v>
       </c>
@@ -27762,7 +27791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:38">
+    <row r="187" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>289</v>
       </c>
@@ -27878,7 +27907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="1:38">
+    <row r="188" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>144</v>
       </c>
@@ -27994,7 +28023,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:38">
+    <row r="189" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>145</v>
       </c>
@@ -28110,7 +28139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:38">
+    <row r="190" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>290</v>
       </c>
@@ -28226,7 +28255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:38">
+    <row r="191" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>146</v>
       </c>
@@ -28342,7 +28371,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:38">
+    <row r="192" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>147</v>
       </c>
@@ -28458,7 +28487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:38">
+    <row r="193" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>148</v>
       </c>
@@ -28574,7 +28603,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="194" spans="1:38">
+    <row r="194" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A194" s="6">
         <v>149</v>
       </c>
@@ -28690,7 +28719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:38">
+    <row r="195" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>150</v>
       </c>
@@ -28806,7 +28835,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="196" spans="1:38">
+    <row r="196" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>151</v>
       </c>
@@ -28922,7 +28951,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="197" spans="1:38">
+    <row r="197" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>152</v>
       </c>
@@ -29038,7 +29067,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:38">
+    <row r="198" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A198" s="6">
         <v>153</v>
       </c>
@@ -29154,7 +29183,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:38">
+    <row r="199" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>291</v>
       </c>
@@ -29270,7 +29299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" spans="1:38">
+    <row r="200" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>292</v>
       </c>
@@ -29386,7 +29415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="1:38">
+    <row r="201" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>293</v>
       </c>
@@ -29502,7 +29531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="1:38">
+    <row r="202" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>154</v>
       </c>
@@ -29618,7 +29647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="1:38">
+    <row r="203" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>294</v>
       </c>
@@ -29734,7 +29763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:38">
+    <row r="204" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>155</v>
       </c>
@@ -29850,7 +29879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="205" spans="1:38">
+    <row r="205" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>156</v>
       </c>
@@ -29966,7 +29995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:38">
+    <row r="206" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>295</v>
       </c>
@@ -30082,7 +30111,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="207" spans="1:38">
+    <row r="207" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>296</v>
       </c>
@@ -30198,7 +30227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="1:38">
+    <row r="208" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>157</v>
       </c>
@@ -30314,7 +30343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="1:38">
+    <row r="209" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>158</v>
       </c>
@@ -30430,7 +30459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" spans="1:38">
+    <row r="210" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>159</v>
       </c>
@@ -30546,7 +30575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:38">
+    <row r="211" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>160</v>
       </c>
@@ -30662,7 +30691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:38">
+    <row r="212" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>161</v>
       </c>
@@ -30778,7 +30807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="213" spans="1:38">
+    <row r="213" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>297</v>
       </c>
@@ -30894,7 +30923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="214" spans="1:38">
+    <row r="214" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>298</v>
       </c>
@@ -31010,7 +31039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="215" spans="1:38">
+    <row r="215" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>162</v>
       </c>
@@ -31126,7 +31155,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="216" spans="1:38">
+    <row r="216" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>299</v>
       </c>
@@ -31242,7 +31271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="217" spans="1:38">
+    <row r="217" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>164</v>
       </c>
@@ -31358,7 +31387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="218" spans="1:38">
+    <row r="218" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>163</v>
       </c>
@@ -31474,7 +31503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="219" spans="1:38">
+    <row r="219" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>165</v>
       </c>
@@ -31590,7 +31619,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="220" spans="1:38">
+    <row r="220" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>168</v>
       </c>
@@ -31706,7 +31735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="221" spans="1:38">
+    <row r="221" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>166</v>
       </c>
@@ -31822,7 +31851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="222" spans="1:38">
+    <row r="222" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>300</v>
       </c>
@@ -31938,7 +31967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="223" spans="1:38">
+    <row r="223" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>301</v>
       </c>
@@ -32054,7 +32083,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="224" spans="1:38">
+    <row r="224" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>167</v>
       </c>
@@ -32170,7 +32199,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="225" spans="1:38">
+    <row r="225" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>169</v>
       </c>
@@ -32286,7 +32315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="226" spans="1:38">
+    <row r="226" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>170</v>
       </c>
@@ -32402,7 +32431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:38">
+    <row r="227" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>171</v>
       </c>
@@ -32518,7 +32547,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="228" spans="1:38">
+    <row r="228" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>303</v>
       </c>
@@ -32634,7 +32663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="229" spans="1:38">
+    <row r="229" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>172</v>
       </c>
@@ -32750,7 +32779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="230" spans="1:38">
+    <row r="230" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>304</v>
       </c>
@@ -32866,7 +32895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="231" spans="1:38">
+    <row r="231" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A231" s="6">
         <v>173</v>
       </c>
@@ -32982,7 +33011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="1:38">
+    <row r="232" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>174</v>
       </c>
@@ -33098,7 +33127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="233" spans="1:38">
+    <row r="233" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>305</v>
       </c>
@@ -33214,7 +33243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="234" spans="1:38">
+    <row r="234" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>8</v>
       </c>
@@ -33327,7 +33356,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="235" spans="1:38">
+    <row r="235" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>175</v>
       </c>
@@ -33443,7 +33472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="236" spans="1:38">
+    <row r="236" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>306</v>
       </c>
@@ -33559,7 +33588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="237" spans="1:38">
+    <row r="237" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>176</v>
       </c>
@@ -33675,7 +33704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="238" spans="1:38">
+    <row r="238" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>177</v>
       </c>
@@ -33791,7 +33820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="239" spans="1:38">
+    <row r="239" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>307</v>
       </c>
@@ -33907,7 +33936,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="240" spans="1:38">
+    <row r="240" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>308</v>
       </c>
@@ -34023,7 +34052,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="241" spans="1:38">
+    <row r="241" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>178</v>
       </c>
@@ -34139,7 +34168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="242" spans="1:38">
+    <row r="242" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>179</v>
       </c>
@@ -34255,7 +34284,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="243" spans="1:38">
+    <row r="243" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>180</v>
       </c>
@@ -34371,7 +34400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="244" spans="1:38">
+    <row r="244" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>181</v>
       </c>
@@ -34379,34 +34408,34 @@
         <v>1033</v>
       </c>
       <c r="C244" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="D244" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E244" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="F244" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="G244" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="H244" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="I244" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="J244" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="K244" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="L244" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="M244" t="s">
         <v>45</v>
@@ -34487,7 +34516,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="245" spans="1:38">
+    <row r="245" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A245" s="6">
         <v>309</v>
       </c>
@@ -34603,7 +34632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="246" spans="1:38">
+    <row r="246" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>182</v>
       </c>
@@ -34719,7 +34748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="247" spans="1:38">
+    <row r="247" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>310</v>
       </c>
@@ -34835,7 +34864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="248" spans="1:38">
+    <row r="248" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>188</v>
       </c>
@@ -34843,34 +34872,34 @@
         <v>1044</v>
       </c>
       <c r="C248" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="D248" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E248" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="F248" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="G248" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="H248" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="I248" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="J248" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="K248" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="L248" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="M248" t="s">
         <v>45</v>
@@ -34951,7 +34980,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="249" spans="1:38">
+    <row r="249" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>189</v>
       </c>
@@ -35067,7 +35096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="250" spans="1:38">
+    <row r="250" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>190</v>
       </c>
@@ -35183,7 +35212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="251" spans="1:38">
+    <row r="251" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>191</v>
       </c>
@@ -35299,7 +35328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="252" spans="1:38">
+    <row r="252" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A252">
         <v>311</v>
       </c>
@@ -35415,7 +35444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="253" spans="1:38">
+    <row r="253" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>192</v>
       </c>
@@ -35528,7 +35557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="254" spans="1:38">
+    <row r="254" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A254">
         <v>312</v>
       </c>
@@ -35644,7 +35673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="255" spans="1:38">
+    <row r="255" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A255" s="6">
         <v>313</v>
       </c>
@@ -35760,7 +35789,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="256" spans="1:38">
+    <row r="256" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A256">
         <v>193</v>
       </c>
@@ -35876,7 +35905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="257" spans="1:38">
+    <row r="257" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A257">
         <v>314</v>
       </c>
@@ -35992,7 +36021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="258" spans="1:38">
+    <row r="258" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A258">
         <v>315</v>
       </c>
@@ -36108,7 +36137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="259" spans="1:38">
+    <row r="259" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A259">
         <v>194</v>
       </c>
@@ -36224,7 +36253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="260" spans="1:38" ht="15.6">
+    <row r="260" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A260">
         <v>196</v>
       </c>
@@ -36340,7 +36369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="261" spans="1:38">
+    <row r="261" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A261">
         <v>197</v>
       </c>
@@ -36456,7 +36485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="262" spans="1:38">
+    <row r="262" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A262">
         <v>198</v>
       </c>
@@ -36572,7 +36601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="263" spans="1:38">
+    <row r="263" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A263">
         <v>199</v>
       </c>
@@ -36580,16 +36609,16 @@
         <v>1091</v>
       </c>
       <c r="C263" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D263" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E263" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="F263" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="G263" t="s">
         <v>45</v>
@@ -36688,7 +36717,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="264" spans="1:38">
+    <row r="264" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A264">
         <v>200</v>
       </c>
@@ -36804,7 +36833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="265" spans="1:38">
+    <row r="265" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A265">
         <v>201</v>
       </c>
@@ -36917,7 +36946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="266" spans="1:38">
+    <row r="266" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A266">
         <v>316</v>
       </c>
@@ -37033,7 +37062,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="267" spans="1:38">
+    <row r="267" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A267">
         <v>202</v>
       </c>
@@ -37149,7 +37178,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="268" spans="1:38">
+    <row r="268" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A268">
         <v>203</v>
       </c>
@@ -37265,7 +37294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="269" spans="1:38">
+    <row r="269" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A269">
         <v>204</v>
       </c>
@@ -37381,7 +37410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="270" spans="1:38">
+    <row r="270" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A270">
         <v>318</v>
       </c>
@@ -37497,7 +37526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="271" spans="1:38">
+    <row r="271" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A271">
         <v>205</v>
       </c>
@@ -37613,7 +37642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="272" spans="1:38">
+    <row r="272" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A272">
         <v>320</v>
       </c>
@@ -37729,7 +37758,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="273" spans="1:38">
+    <row r="273" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A273">
         <v>321</v>
       </c>
@@ -37845,7 +37874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="274" spans="1:38">
+    <row r="274" spans="1:38" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A274">
         <v>206</v>
       </c>
@@ -37961,7 +37990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="275" spans="1:38">
+    <row r="275" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A275">
         <v>322</v>
       </c>
@@ -38077,7 +38106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="276" spans="1:38">
+    <row r="276" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A276">
         <v>207</v>
       </c>
@@ -38193,7 +38222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="277" spans="1:38">
+    <row r="277" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A277">
         <v>208</v>
       </c>
@@ -38309,7 +38338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="278" spans="1:38">
+    <row r="278" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A278">
         <v>323</v>
       </c>
@@ -38425,7 +38454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="279" spans="1:38">
+    <row r="279" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A279">
         <v>209</v>
       </c>
@@ -38541,7 +38570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="280" spans="1:38">
+    <row r="280" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A280">
         <v>210</v>
       </c>
@@ -38657,7 +38686,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="281" spans="1:38">
+    <row r="281" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A281" s="6">
         <v>211</v>
       </c>
@@ -38773,7 +38802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="282" spans="1:38">
+    <row r="282" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A282">
         <v>324</v>
       </c>
@@ -38889,7 +38918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="283" spans="1:38">
+    <row r="283" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A283">
         <v>212</v>
       </c>
@@ -39005,7 +39034,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="284" spans="1:38">
+    <row r="284" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A284">
         <v>213</v>
       </c>
@@ -39121,7 +39150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="285" spans="1:38">
+    <row r="285" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A285">
         <v>215</v>
       </c>
@@ -39237,7 +39266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="286" spans="1:38">
+    <row r="286" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A286">
         <v>214</v>
       </c>
@@ -39353,7 +39382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="287" spans="1:38">
+    <row r="287" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A287">
         <v>216</v>
       </c>
@@ -39469,7 +39498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="288" spans="1:38">
+    <row r="288" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A288">
         <v>217</v>
       </c>
@@ -39585,7 +39614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="289" spans="1:38">
+    <row r="289" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A289">
         <v>219</v>
       </c>
@@ -39701,7 +39730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="290" spans="1:38">
+    <row r="290" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A290">
         <v>220</v>
       </c>
@@ -39817,7 +39846,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="291" spans="1:38">
+    <row r="291" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A291">
         <v>221</v>
       </c>
@@ -39933,7 +39962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="292" spans="1:38">
+    <row r="292" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A292">
         <v>222</v>
       </c>
@@ -40049,7 +40078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="293" spans="1:38">
+    <row r="293" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A293">
         <v>223</v>
       </c>
@@ -40165,7 +40194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="294" spans="1:38">
+    <row r="294" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A294">
         <v>325</v>
       </c>
@@ -40281,7 +40310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="295" spans="1:38">
+    <row r="295" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A295" s="6">
         <v>224</v>
       </c>
@@ -40397,7 +40426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="296" spans="1:38">
+    <row r="296" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A296">
         <v>327</v>
       </c>
@@ -40513,7 +40542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="297" spans="1:38">
+    <row r="297" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A297">
         <v>328</v>
       </c>
@@ -40629,7 +40658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="298" spans="1:38">
+    <row r="298" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A298">
         <v>225</v>
       </c>
@@ -40745,7 +40774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="299" spans="1:38">
+    <row r="299" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A299" s="6">
         <v>329</v>
       </c>
@@ -40861,7 +40890,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="300" spans="1:38">
+    <row r="300" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A300">
         <v>226</v>
       </c>
@@ -40977,7 +41006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="301" spans="1:38">
+    <row r="301" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A301">
         <v>330</v>
       </c>
@@ -41093,7 +41122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="302" spans="1:38">
+    <row r="302" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A302">
         <v>229</v>
       </c>
@@ -41209,7 +41238,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="303" spans="1:38">
+    <row r="303" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A303">
         <v>230</v>
       </c>
@@ -41325,7 +41354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="304" spans="1:38">
+    <row r="304" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A304">
         <v>232</v>
       </c>
@@ -41441,7 +41470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="305" spans="1:38">
+    <row r="305" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A305">
         <v>233</v>
       </c>
@@ -41557,7 +41586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="306" spans="1:38">
+    <row r="306" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A306">
         <v>234</v>
       </c>
@@ -41673,7 +41702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="307" spans="1:38">
+    <row r="307" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A307">
         <v>235</v>
       </c>
@@ -41789,7 +41818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="308" spans="1:38">
+    <row r="308" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A308">
         <v>236</v>
       </c>
@@ -41905,7 +41934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="309" spans="1:38">
+    <row r="309" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A309">
         <v>237</v>
       </c>
@@ -42021,7 +42050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="310" spans="1:38">
+    <row r="310" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A310">
         <v>332</v>
       </c>
@@ -42137,7 +42166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="311" spans="1:38">
+    <row r="311" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A311">
         <v>238</v>
       </c>
@@ -42253,7 +42282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="312" spans="1:38">
+    <row r="312" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A312">
         <v>239</v>
       </c>
@@ -42369,7 +42398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="313" spans="1:38" ht="20.399999999999999">
+    <row r="313" spans="1:38" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A313" s="6">
         <v>240</v>
       </c>
@@ -42485,7 +42514,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="314" spans="1:38">
+    <row r="314" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A314">
         <v>242</v>
       </c>
@@ -42601,7 +42630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="315" spans="1:38">
+    <row r="315" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A315">
         <v>243</v>
       </c>
@@ -42717,7 +42746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="316" spans="1:38">
+    <row r="316" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A316">
         <v>333</v>
       </c>
@@ -42740,16 +42769,16 @@
         <v>1699</v>
       </c>
       <c r="H316" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="I316" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="J316" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="K316" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="L316" s="3" t="s">
         <v>1698</v>
@@ -42833,7 +42862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="317" spans="1:38">
+    <row r="317" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A317">
         <v>244</v>
       </c>
@@ -42841,16 +42870,16 @@
         <v>1266</v>
       </c>
       <c r="C317" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D317" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E317" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="F317" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="G317" t="s">
         <v>45</v>
@@ -42949,7 +42978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="318" spans="1:38">
+    <row r="318" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A318">
         <v>245</v>
       </c>
@@ -43065,7 +43094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="319" spans="1:38">
+    <row r="319" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A319">
         <v>246</v>
       </c>
@@ -43181,7 +43210,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="320" spans="1:38">
+    <row r="320" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A320">
         <v>334</v>
       </c>
@@ -43297,7 +43326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="321" spans="1:38">
+    <row r="321" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A321">
         <v>247</v>
       </c>
@@ -43413,7 +43442,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="322" spans="1:38">
+    <row r="322" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A322">
         <v>335</v>
       </c>
@@ -43529,7 +43558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="323" spans="1:38">
+    <row r="323" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A323">
         <v>248</v>
       </c>
@@ -43645,7 +43674,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="324" spans="1:38">
+    <row r="324" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A324">
         <v>228</v>
       </c>
@@ -43761,7 +43790,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="325" spans="1:38">
+    <row r="325" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A325">
         <v>15</v>
       </c>
@@ -43877,7 +43906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="326" spans="1:38">
+    <row r="326" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A326">
         <v>249</v>
       </c>
@@ -43993,7 +44022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="327" spans="1:38">
+    <row r="327" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A327">
         <v>336</v>
       </c>
@@ -44109,7 +44138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="328" spans="1:38">
+    <row r="328" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A328">
         <v>337</v>
       </c>
@@ -44225,7 +44254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="329" spans="1:38">
+    <row r="329" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A329">
         <v>123</v>
       </c>
@@ -44341,7 +44370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="330" spans="1:38">
+    <row r="330" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A330">
         <v>185</v>
       </c>
@@ -44457,7 +44486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="331" spans="1:38">
+    <row r="331" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A331">
         <v>186</v>
       </c>
@@ -44573,7 +44602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="332" spans="1:38">
+    <row r="332" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A332">
         <v>241</v>
       </c>
@@ -44688,77 +44717,78 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K97" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="K103" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="G105" r:id="rId3" display="http://www.oalib.com/journal/6879/1" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="G108" r:id="rId4" display="https://link.springer.com/book/10.1007/978-1-4471-4072-6" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="K120" r:id="rId5" display="http://citeseerx.ist.psu.edu/viewdoc/summary?doi=10.1.1.101.9163; " xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="G121" r:id="rId6" display="https://leitir.is/primo_library/libweb/action/dlDisplay.do?vid=GEGNIR&amp;docId=ICE01_PRIMO000599234" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="K121" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="I129" r:id="rId8" display="http://repository.unhas.ac.id/" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="K130" r:id="rId9" display="https://www.semanticscholar.org/paper/An-analysis-of-data-characteristics-that-affect-RISH-COM/10fd83b0a0ee37b2161e0e98135470c230d513b9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="K131" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="G132" r:id="rId11" tooltip="Current Pharmacology Reports" display="https://link.springer.com/journal/40495" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="G135" r:id="rId12" tooltip="European Radiology" display="https://link.springer.com/journal/330" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="L137" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="G143" r:id="rId14" display="https://link.springer.com/conference/icics" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="G146" r:id="rId15" tooltip="Conference Website" display="http://chi2012.acm.org/" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="L146" r:id="rId16" display="https://doi.org/10.1145/2207676.2208640" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="L148" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="L160" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="J160" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="L170" r:id="rId20" display="https://doi.org/10.1177%2F1555412010364981" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="L186" r:id="rId21" display="https://doi.org/10.1109/CONIELECOMP.2012.6189918" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="K197" r:id="rId22" display="https://pdfs.semanticscholar.org/cec0/ad7b0fc2d4d6ba45c6212d36217df1ff2bf2.pdf;http://citeseerx.ist.psu.edu/viewdoc/summary?doi=10.1.1.55.9568" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="L200" r:id="rId23" tooltip="Persistent link using digital object identifier" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="G208" r:id="rId24" display="https://app.dimensions.ai/discover/publication?and_facet_journal=jour.1083795" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="K208" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="L212" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="G212" r:id="rId27" tooltip="link to all content in Journal of Medical Imaging and Health Informatics" display="https://www.ingentaconnect.com/content/asp/jmihi" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="K213" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="G213" r:id="rId29" display="https://ieeexplore.ieee.org/xpl/mostRecentIssue.jsp?punumber=6679357" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="G219" r:id="rId30" tooltip="Waste and Biomass Valorization" display="https://link.springer.com/journal/12649" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="L222" r:id="rId31" display="https://doi.org/10.1109/MCOM.2010.5673086" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="G222" r:id="rId32" display="https://ieeexplore.ieee.org/xpl/RecentIssue.jsp?punumber=35" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="L223" r:id="rId33" tooltip="Persistent link using digital object identifier" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="G228" r:id="rId34" display="https://library.seg.org/doi/book/10.1190/SEGEAB.19" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="L228" r:id="rId35" tooltip="Opens new window" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="L234" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="K237" r:id="rId37" display="http://cdn.iiit.ac.in/cdn/speech.iiit.ac.in/svlpubs/conference/Kishore2002a.pdf" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="G253" r:id="rId38" display="https://findit.dtu.dk/en/journal?ignore_search=%E2%9C%93&amp;issn%5B%5D=19422601&amp;key=19422601%7C000088%7C000004%7C000003%7C000000" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="J257" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="L258" r:id="rId40" display="https://doi.org/10.1177%2F1528083714532113" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="L269" r:id="rId41" tooltip="Persistent link using digital object identifier" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="G272" r:id="rId42" display="https://ukm.pure.elsevier.com/en/publications/heuristic-optimization-techniques-to-determine-optimal-capacitor-" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="L282" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="K283" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="L284" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="L286" r:id="rId46" display="https://doi.org/10.1109/SECON.2009.5174082" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="L291" r:id="rId47" tooltip="Persistent link using digital object identifier" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="L293" r:id="rId48" tooltip="Persistent link using digital object identifier" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="K297" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="L300" r:id="rId50" display="https://doi.org/10.1109/NUICONE.2015.7449639" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="G300" r:id="rId51" display="https://ieeexplore.ieee.org/xpl/mostRecentIssue.jsp?punumber=7446021" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="L301" r:id="rId52" display="https://doi.org/10.1109/IECON.2013.6699111" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="G302" r:id="rId53" tooltip="Conference Website" display="https://www.acm.org/conferences/sac/sac2015/" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="L302" r:id="rId54" display="https://doi.org/10.1145/2695664.2695719" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="L304" r:id="rId55" tooltip="Persistent link using digital object identifier" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="G307" r:id="rId56" display="http://journaldatabase.info/journal/issn2229-6093" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
-    <hyperlink ref="L311" r:id="rId57" display="https://doi.org/10.1109/WHISPERS.2014.8077520" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="L312" r:id="rId58" display="https://dx.doi.org/10.1016%2Fj.trstmh.2010.09.007" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="L316" r:id="rId59" tooltip="Persistent link using digital object identifier" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="L318" r:id="rId60" tooltip="Persistent link using digital object identifier" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="G320" r:id="rId61" display="https://www.igi-global.com/book/big-data-management-technologies-applications/77404" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="G321" r:id="rId62" display="https://link.springer.com/referencework/10.1007/978-94-007-6064-6" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="G322" r:id="rId63" display="https://ieeexplore.ieee.org/xpl/mostRecentIssue.jsp?punumber=9626" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="L322" r:id="rId64" display="https://doi.org/10.1109/ACSSC.2004.1399438" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="J323" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="L326" r:id="rId66" display="https://doi.org/10.1145/2030112.2030127" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="K255" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
-    <hyperlink ref="J299" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="K299" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="K97" r:id="rId1"/>
+    <hyperlink ref="K103" r:id="rId2"/>
+    <hyperlink ref="G105" r:id="rId3" display="http://www.oalib.com/journal/6879/1"/>
+    <hyperlink ref="G108" r:id="rId4" display="https://link.springer.com/book/10.1007/978-1-4471-4072-6"/>
+    <hyperlink ref="K120" r:id="rId5" display="http://citeseerx.ist.psu.edu/viewdoc/summary?doi=10.1.1.101.9163; "/>
+    <hyperlink ref="G121" r:id="rId6" display="https://leitir.is/primo_library/libweb/action/dlDisplay.do?vid=GEGNIR&amp;docId=ICE01_PRIMO000599234"/>
+    <hyperlink ref="K121" r:id="rId7"/>
+    <hyperlink ref="I129" r:id="rId8" display="http://repository.unhas.ac.id/"/>
+    <hyperlink ref="K130" r:id="rId9" display="https://www.semanticscholar.org/paper/An-analysis-of-data-characteristics-that-affect-RISH-COM/10fd83b0a0ee37b2161e0e98135470c230d513b9"/>
+    <hyperlink ref="K131" r:id="rId10"/>
+    <hyperlink ref="G132" r:id="rId11" tooltip="Current Pharmacology Reports" display="https://link.springer.com/journal/40495"/>
+    <hyperlink ref="G135" r:id="rId12" tooltip="European Radiology" display="https://link.springer.com/journal/330"/>
+    <hyperlink ref="L137" r:id="rId13"/>
+    <hyperlink ref="G143" r:id="rId14" display="https://link.springer.com/conference/icics"/>
+    <hyperlink ref="G146" r:id="rId15" tooltip="Conference Website" display="http://chi2012.acm.org/"/>
+    <hyperlink ref="L146" r:id="rId16" display="https://doi.org/10.1145/2207676.2208640"/>
+    <hyperlink ref="L148" r:id="rId17"/>
+    <hyperlink ref="L160" r:id="rId18"/>
+    <hyperlink ref="J160" r:id="rId19"/>
+    <hyperlink ref="L170" r:id="rId20" display="https://doi.org/10.1177%2F1555412010364981"/>
+    <hyperlink ref="L186" r:id="rId21" display="https://doi.org/10.1109/CONIELECOMP.2012.6189918"/>
+    <hyperlink ref="K197" r:id="rId22" display="https://pdfs.semanticscholar.org/cec0/ad7b0fc2d4d6ba45c6212d36217df1ff2bf2.pdf;http://citeseerx.ist.psu.edu/viewdoc/summary?doi=10.1.1.55.9568"/>
+    <hyperlink ref="L200" r:id="rId23" tooltip="Persistent link using digital object identifier"/>
+    <hyperlink ref="G208" r:id="rId24" display="https://app.dimensions.ai/discover/publication?and_facet_journal=jour.1083795"/>
+    <hyperlink ref="K208" r:id="rId25"/>
+    <hyperlink ref="L212" r:id="rId26"/>
+    <hyperlink ref="G212" r:id="rId27" tooltip="link to all content in Journal of Medical Imaging and Health Informatics" display="https://www.ingentaconnect.com/content/asp/jmihi"/>
+    <hyperlink ref="K213" r:id="rId28"/>
+    <hyperlink ref="G213" r:id="rId29" display="https://ieeexplore.ieee.org/xpl/mostRecentIssue.jsp?punumber=6679357"/>
+    <hyperlink ref="G219" r:id="rId30" tooltip="Waste and Biomass Valorization" display="https://link.springer.com/journal/12649"/>
+    <hyperlink ref="L222" r:id="rId31" display="https://doi.org/10.1109/MCOM.2010.5673086"/>
+    <hyperlink ref="G222" r:id="rId32" display="https://ieeexplore.ieee.org/xpl/RecentIssue.jsp?punumber=35"/>
+    <hyperlink ref="L223" r:id="rId33" tooltip="Persistent link using digital object identifier"/>
+    <hyperlink ref="G228" r:id="rId34" display="https://library.seg.org/doi/book/10.1190/SEGEAB.19"/>
+    <hyperlink ref="L228" r:id="rId35" tooltip="Opens new window"/>
+    <hyperlink ref="L234" r:id="rId36"/>
+    <hyperlink ref="K237" r:id="rId37" display="http://cdn.iiit.ac.in/cdn/speech.iiit.ac.in/svlpubs/conference/Kishore2002a.pdf"/>
+    <hyperlink ref="G253" r:id="rId38" display="https://findit.dtu.dk/en/journal?ignore_search=%E2%9C%93&amp;issn%5B%5D=19422601&amp;key=19422601%7C000088%7C000004%7C000003%7C000000"/>
+    <hyperlink ref="J257" r:id="rId39"/>
+    <hyperlink ref="L258" r:id="rId40" display="https://doi.org/10.1177%2F1528083714532113"/>
+    <hyperlink ref="L269" r:id="rId41" tooltip="Persistent link using digital object identifier"/>
+    <hyperlink ref="G272" r:id="rId42" display="https://ukm.pure.elsevier.com/en/publications/heuristic-optimization-techniques-to-determine-optimal-capacitor-"/>
+    <hyperlink ref="L282" r:id="rId43"/>
+    <hyperlink ref="K283" r:id="rId44"/>
+    <hyperlink ref="L284" r:id="rId45"/>
+    <hyperlink ref="L286" r:id="rId46" display="https://doi.org/10.1109/SECON.2009.5174082"/>
+    <hyperlink ref="L291" r:id="rId47" tooltip="Persistent link using digital object identifier"/>
+    <hyperlink ref="L293" r:id="rId48" tooltip="Persistent link using digital object identifier"/>
+    <hyperlink ref="K297" r:id="rId49"/>
+    <hyperlink ref="L300" r:id="rId50" display="https://doi.org/10.1109/NUICONE.2015.7449639"/>
+    <hyperlink ref="G300" r:id="rId51" display="https://ieeexplore.ieee.org/xpl/mostRecentIssue.jsp?punumber=7446021"/>
+    <hyperlink ref="L301" r:id="rId52" display="https://doi.org/10.1109/IECON.2013.6699111"/>
+    <hyperlink ref="G302" r:id="rId53" tooltip="Conference Website" display="https://www.acm.org/conferences/sac/sac2015/"/>
+    <hyperlink ref="L302" r:id="rId54" display="https://doi.org/10.1145/2695664.2695719"/>
+    <hyperlink ref="L304" r:id="rId55" tooltip="Persistent link using digital object identifier"/>
+    <hyperlink ref="G307" r:id="rId56" display="http://journaldatabase.info/journal/issn2229-6093"/>
+    <hyperlink ref="L311" r:id="rId57" display="https://doi.org/10.1109/WHISPERS.2014.8077520"/>
+    <hyperlink ref="L312" r:id="rId58" display="https://dx.doi.org/10.1016%2Fj.trstmh.2010.09.007"/>
+    <hyperlink ref="L316" r:id="rId59" tooltip="Persistent link using digital object identifier"/>
+    <hyperlink ref="L318" r:id="rId60" tooltip="Persistent link using digital object identifier"/>
+    <hyperlink ref="G320" r:id="rId61" display="https://www.igi-global.com/book/big-data-management-technologies-applications/77404"/>
+    <hyperlink ref="G321" r:id="rId62" display="https://link.springer.com/referencework/10.1007/978-94-007-6064-6"/>
+    <hyperlink ref="G322" r:id="rId63" display="https://ieeexplore.ieee.org/xpl/mostRecentIssue.jsp?punumber=9626"/>
+    <hyperlink ref="L322" r:id="rId64" display="https://doi.org/10.1109/ACSSC.2004.1399438"/>
+    <hyperlink ref="J323" r:id="rId65"/>
+    <hyperlink ref="L326" r:id="rId66" display="https://doi.org/10.1145/2030112.2030127"/>
+    <hyperlink ref="K255" r:id="rId67"/>
+    <hyperlink ref="J299" r:id="rId68"/>
+    <hyperlink ref="K299" r:id="rId69"/>
+    <hyperlink ref="K145" r:id="rId70"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId70"/>
+  <pageSetup orientation="portrait" r:id="rId71"/>
 </worksheet>
 </file>
</xml_diff>